<commit_message>
Testcase form chi tiết
</commit_message>
<xml_diff>
--- a/My test/Test CNPM/Where_Index.xlsx
+++ b/My test/Test CNPM/Where_Index.xlsx
@@ -4,20 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Chi tiết bài viết" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="260">
   <si>
     <t>System</t>
   </si>
@@ -680,6 +679,297 @@
   </si>
   <si>
     <t>Kiểm tra chức năng phần content</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Màn chi tiết bài viết:
+ -  Kiểm tra về bố cục, font chữ, chính tả, màu chữ, màu nền</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Màn chi tiết bài viết:
+ - Kiểm tra title của màn hình
+ - Kiểm tra các giá trị mặc định của các trường, button
+ - Kiểm tra việc hiển thị các icon</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Màn chi tiết bài viết:
+- Nhấn Tab liên tục</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Màn chi tiết bài viết:
+- Nhấn phím Shift-Tab liên tục</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Màn chi tiết bài viết:
+- Nhấn phím Ctrl -
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Màn chi tiết bài viết:
+ - Nhấn phim Ctrl +</t>
+  </si>
+  <si>
+    <t>Kiểm tra chức năng phẩn header</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Màn chi tiết bài viết:
+- Kiểm tra giá trị mặc định khi khởi tạo header</t>
+  </si>
+  <si>
+    <t>Bao gồm:
+- Ảnh
+- Tên địa điểm
+- Lượt thích
+-Giới thiệu địa điểm
+- Button [Chơi luôn]</t>
+  </si>
+  <si>
+    <t>Button [Chơi luôn]</t>
+  </si>
+  <si>
+    <t>Kiểm tra giá trị mặc định khi khởi tạo của button [Chơi luôn]</t>
+  </si>
+  <si>
+    <t>Kiểm tra sự kiện khi hover chuột vào button [Chơi luôn]</t>
+  </si>
+  <si>
+    <t>Kiểm tra sự kiện khi click chuột vào button [Chơi luôn]</t>
+  </si>
+  <si>
+    <t>Con trỏ chuột hiển thị hình bàn tay
+Button chuyển thành màu xám</t>
+  </si>
+  <si>
+    <t>Chuyển sang trang tạo lịch trình</t>
+  </si>
+  <si>
+    <t>Thanh menu</t>
+  </si>
+  <si>
+    <t>Màn chi tiết bài viết:
+- Kiểm tra giá trị mặc định khi khởi tạo button [Chơi luôn]</t>
+  </si>
+  <si>
+    <t>Màn chi tiết bài viết:
+- Hover chuột vào button [Chơi luôn]</t>
+  </si>
+  <si>
+    <t>Màn chi tiết bài viết:
+- Click chuột vào button [Chơi luôn]</t>
+  </si>
+  <si>
+    <t>Màn chi tiết bài viết:
+- Kiểm tra giá trị mặc định khi khởi tạo thanh menu</t>
+  </si>
+  <si>
+    <t>Không hiển thị thanh menu</t>
+  </si>
+  <si>
+    <t>Màn chi tiết bài viết:
+- Scroll xuống dưới
+- Kiểm tra giá trị mặc định khi khởi tạo thanh menu</t>
+  </si>
+  <si>
+    <t>Hiểm thị thanh menu gồm :
+- Logo
+- Link [Đăng nhâp]</t>
+  </si>
+  <si>
+    <t>Logo</t>
+  </si>
+  <si>
+    <t>Màn chi tiết bài viết:
+- Click chuột vào logo</t>
+  </si>
+  <si>
+    <t>Kiểm tra sự kiện khi hover chuột vào logo</t>
+  </si>
+  <si>
+    <t>Kiểm tra sự kiện khi click chuột vào logo</t>
+  </si>
+  <si>
+    <t>Màn chi tiết bài viết:
+- Hover chuột vào logo</t>
+  </si>
+  <si>
+    <t>Trở về trang chính</t>
+  </si>
+  <si>
+    <t>Link [Đăng nhâp]</t>
+  </si>
+  <si>
+    <t>Kiểm tra giá trị mặc định khi khởi tạo của Link [Đăng nhâp]</t>
+  </si>
+  <si>
+    <t>Kiểm tra sự kiện khi hover chuột vào Link [Đăng nhâp]</t>
+  </si>
+  <si>
+    <t>Kiểm tra sự kiện khi click chuột vào Link [Đăng nhâp]</t>
+  </si>
+  <si>
+    <t>Màn chi tiết bài viết:
+- Hover chuột vào Link [Đăng nhâp]</t>
+  </si>
+  <si>
+    <t>Màn chi tiết bài viết:
+- Click chuột vào Link [Đăng nhâp]</t>
+  </si>
+  <si>
+    <t>Màn chi tiết bài viết:
+- Kiểm tra giá trị mặc định khi khởi tạo Link [Đăng nhâp]</t>
+  </si>
+  <si>
+    <t>Chuữ màu xanh</t>
+  </si>
+  <si>
+    <t>Màn chi tiết bài viết:
+- Kiểm tra giá trị mặc định khi khởi tạo button [Facebook]</t>
+  </si>
+  <si>
+    <t>Màn chi tiết bài viết:
+- Hover chuột vào button [Facebook]</t>
+  </si>
+  <si>
+    <t>Màn chi tiết bài viết:
+- Click chuột vào button [Facebook]</t>
+  </si>
+  <si>
+    <t>Màn chi tiết bài viết:
+- Kiểm tra giá trị mặc định khi khởi tạo button [Google+]</t>
+  </si>
+  <si>
+    <t>Màn chi tiết bài viết:
+- Hover chuột vào button [Google+]</t>
+  </si>
+  <si>
+    <t>Màn chi tiết bài viết:
+- Click chuột vào button [Google+]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Màn chi tiết bài viết:
+- Kiểm tra giá trị mặc định khi khởi tạo content</t>
+  </si>
+  <si>
+    <t>Slide show</t>
+  </si>
+  <si>
+    <t>Kiểm tra giá trị mặc định khi khởi tạo của Slide show</t>
+  </si>
+  <si>
+    <t>Màn chi tiết bài viết:
+- Kiểm tra giá trị mặc định khi khởi tạo Slide show</t>
+  </si>
+  <si>
+    <t>Bao gồm:
+- 1 ảnh to
+- 5 ảnh nhỏ phía dưới
+- Ảnh trượt sang ngang để chuyển ảnh</t>
+  </si>
+  <si>
+    <t>Link bài viết liên quan</t>
+  </si>
+  <si>
+    <t>Kiểm tra sự kiện khi hover chuột vào link</t>
+  </si>
+  <si>
+    <t>Kiểm tra sự kiện khi click chuột vào link</t>
+  </si>
+  <si>
+    <t>Màn chi tiết bài viết:
+- Hover chuột vào link</t>
+  </si>
+  <si>
+    <t>Màn chi tiết bài viết:
+- Click chuột vào link</t>
+  </si>
+  <si>
+    <t>Con trỏ chuột hiển thị hình bàn tay
+Có gạch chân chữ</t>
+  </si>
+  <si>
+    <t>Chuyển sang trang bài viết</t>
+  </si>
+  <si>
+    <t>Bản đồ</t>
+  </si>
+  <si>
+    <t>Kiểm tra sự kiện khi click chuột vào bản đồ</t>
+  </si>
+  <si>
+    <t>Màn chi tiết bài viết:
+- click chuột vào 1 điểm bất kỳ bản đồ</t>
+  </si>
+  <si>
+    <t>Hiển thị địa chỉ địa điểm đó phía dưới</t>
+  </si>
+  <si>
+    <t>Button [Tính khoảng cách]</t>
+  </si>
+  <si>
+    <t>Kiểm tra giá trị mặc định khi khởi tạo của button [Tính khoảng cách]</t>
+  </si>
+  <si>
+    <t>Kiểm tra sự kiện khi click chuột vào button  [Tính khoảng cách]</t>
+  </si>
+  <si>
+    <t>Kiểm tra sự kiện khi hover chuột vào button [Tính khoảng cách]</t>
+  </si>
+  <si>
+    <t>Màn chi tiết bài viết:
+- Kiểm tra giá trị mặc định khi khởi tạo button  [Tính khoảng cách]</t>
+  </si>
+  <si>
+    <t>Màn chi tiết bài viết:
+- Hover chuột vào button  [Tính khoảng cách]</t>
+  </si>
+  <si>
+    <t>Màn chi tiết bài viết:
+- Click chuột vào button  [Tính khoảng cách]</t>
+  </si>
+  <si>
+    <t>Hiện khoảng cách từ điểm chọn tới điểm đến trên bản đồ</t>
+  </si>
+  <si>
+    <t>Button mày trắng
+Chữ mài đen</t>
+  </si>
+  <si>
+    <t>Con trỏ chuột hiển thị hình bàn tay
+Button chuyển thành màu xám
+Chữ chuyển màu trắng</t>
+  </si>
+  <si>
+    <t>Bao gồm :
+- Têu đề bài viết
+- Địa chỉ bài viết
+- Giới thiệu bài viết
+- Slide show
+- Link bài viết liên quan
+- Button [Đi thôi]
+- bản đồ
+- Địa chỉ điểm đến
+- Địa chỉ lựa chọn
+- Button [tính khoảng cách]
+- Button [Lịch trình của bạn]
+- Một số điểm du lịch khác</t>
+  </si>
+  <si>
+    <t>Một số điểm du lịch khác</t>
+  </si>
+  <si>
+    <t>Màn chi tiết bài viết:
+- Kiểm tra giá trị mặc định khi khởi tạo</t>
+  </si>
+  <si>
+    <t>Bao gồm:
+- Tiêu đề
+- Địa chỉ
+- Ảnh
+- Lượt xem
+- Lượt thích
+- Button [Chi tiết]</t>
+  </si>
+  <si>
+    <t>Button [chi tiết]</t>
   </si>
 </sst>
 </file>
@@ -924,7 +1214,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1016,33 +1306,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1058,27 +1321,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1090,6 +1359,37 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1401,9 +1701,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A63" sqref="A63:XFD64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1436,57 +1736,57 @@
       <c r="Q1" s="5"/>
     </row>
     <row r="2" spans="1:17" s="8" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="39" t="s">
+      <c r="B2" s="52"/>
+      <c r="C2" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="41"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="55"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
       <c r="Q2" s="9"/>
     </row>
     <row r="3" spans="1:17" s="8" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="41"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="55"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="Q3" s="9"/>
     </row>
     <row r="4" spans="1:17" s="8" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="41"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="55"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="Q4" s="9"/>
     </row>
     <row r="5" spans="1:17" s="8" customFormat="1">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="38"/>
+      <c r="B5" s="52"/>
       <c r="C5" s="10" t="s">
         <v>7</v>
       </c>
@@ -1504,8 +1804,8 @@
       <c r="Q5" s="9"/>
     </row>
     <row r="6" spans="1:17" s="20" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A6" s="38"/>
-      <c r="B6" s="38"/>
+      <c r="A6" s="52"/>
+      <c r="B6" s="52"/>
       <c r="C6" s="15">
         <f>COUNTIF(P10:P64,"OK")</f>
         <v>0</v>
@@ -1546,90 +1846,90 @@
       <c r="Q7" s="28"/>
     </row>
     <row r="8" spans="1:17" s="6" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="33" t="s">
+      <c r="B8" s="41"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="37" t="s">
+      <c r="F8" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="35" t="s">
+      <c r="G8" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="36"/>
-      <c r="I8" s="36"/>
-      <c r="J8" s="36"/>
-      <c r="K8" s="36"/>
-      <c r="L8" s="36"/>
-      <c r="M8" s="37"/>
-      <c r="N8" s="33" t="s">
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="46"/>
+      <c r="M8" s="47"/>
+      <c r="N8" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="O8" s="33" t="s">
+      <c r="O8" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="P8" s="33" t="s">
+      <c r="P8" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="Q8" s="34" t="s">
+      <c r="Q8" s="42" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="6" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A9" s="33"/>
-      <c r="B9" s="42" t="s">
+    <row r="9" spans="1:17" s="6" customFormat="1" ht="16.5" customHeight="1">
+      <c r="A9" s="41"/>
+      <c r="B9" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="C9" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="44" t="s">
+      <c r="D9" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="33"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="43" t="s">
+      <c r="E9" s="41"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="H9" s="43" t="s">
+      <c r="H9" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="I9" s="45" t="s">
+      <c r="I9" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="J9" s="45" t="s">
+      <c r="J9" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="K9" s="45" t="s">
+      <c r="K9" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="L9" s="45" t="s">
+      <c r="L9" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="M9" s="45" t="s">
+      <c r="M9" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="N9" s="33"/>
-      <c r="O9" s="33"/>
-      <c r="P9" s="33"/>
-      <c r="Q9" s="34"/>
-    </row>
-    <row r="10" spans="1:17" s="49" customFormat="1" ht="99.75">
-      <c r="A10" s="46">
+      <c r="N9" s="41"/>
+      <c r="O9" s="41"/>
+      <c r="P9" s="41"/>
+      <c r="Q9" s="42"/>
+    </row>
+    <row r="10" spans="1:17" s="38" customFormat="1" ht="99.75">
+      <c r="A10" s="37">
         <v>1</v>
       </c>
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="48" t="s">
+      <c r="C10" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="48"/>
+      <c r="D10" s="44"/>
       <c r="E10" s="30" t="s">
         <v>67</v>
       </c>
@@ -1637,47 +1937,47 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="49" customFormat="1" ht="85.5">
-      <c r="A11" s="46">
+    <row r="11" spans="1:17" s="38" customFormat="1" ht="85.5">
+      <c r="A11" s="37">
         <v>2</v>
       </c>
-      <c r="B11" s="47"/>
-      <c r="C11" s="48" t="s">
+      <c r="B11" s="43"/>
+      <c r="C11" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="48"/>
+      <c r="D11" s="44"/>
       <c r="E11" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="F11" s="46" t="s">
+      <c r="F11" s="37" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="49" customFormat="1" ht="28.5">
-      <c r="A12" s="46">
+    <row r="12" spans="1:17" s="38" customFormat="1" ht="28.5">
+      <c r="A12" s="37">
         <v>3</v>
       </c>
-      <c r="B12" s="47"/>
-      <c r="C12" s="48" t="s">
+      <c r="B12" s="43"/>
+      <c r="C12" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="48"/>
+      <c r="D12" s="44"/>
       <c r="E12" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="F12" s="50" t="s">
+      <c r="F12" s="39" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="49" customFormat="1" ht="28.5">
-      <c r="A13" s="46">
+    <row r="13" spans="1:17" s="38" customFormat="1" ht="28.5">
+      <c r="A13" s="37">
         <v>4</v>
       </c>
-      <c r="B13" s="47"/>
-      <c r="C13" s="48" t="s">
+      <c r="B13" s="43"/>
+      <c r="C13" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="48"/>
+      <c r="D13" s="44"/>
       <c r="E13" s="32" t="s">
         <v>70</v>
       </c>
@@ -1685,15 +1985,15 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="49" customFormat="1" ht="42.75">
-      <c r="A14" s="46">
+    <row r="14" spans="1:17" s="38" customFormat="1" ht="42.75">
+      <c r="A14" s="37">
         <v>5</v>
       </c>
-      <c r="B14" s="47"/>
-      <c r="C14" s="48" t="s">
+      <c r="B14" s="43"/>
+      <c r="C14" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="48"/>
+      <c r="D14" s="44"/>
       <c r="E14" s="32" t="s">
         <v>71</v>
       </c>
@@ -1701,793 +2001,793 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="49" customFormat="1" ht="28.5">
-      <c r="A15" s="46">
+    <row r="15" spans="1:17" s="38" customFormat="1" ht="28.5">
+      <c r="A15" s="37">
         <v>6</v>
       </c>
-      <c r="B15" s="47"/>
-      <c r="C15" s="48" t="s">
+      <c r="B15" s="43"/>
+      <c r="C15" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="48"/>
+      <c r="D15" s="44"/>
       <c r="E15" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="F15" s="50" t="s">
+      <c r="F15" s="39" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="51" customFormat="1" ht="15" customHeight="1">
-      <c r="A16" s="51" t="s">
+    <row r="16" spans="1:17" s="57" customFormat="1" ht="15" customHeight="1">
+      <c r="A16" s="57" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="49" customFormat="1" ht="75">
-      <c r="A17" s="46">
+    <row r="17" spans="1:6" s="38" customFormat="1" ht="75">
+      <c r="A17" s="37">
         <v>7</v>
       </c>
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="C17" s="52" t="s">
+      <c r="C17" s="59" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="52"/>
+      <c r="D17" s="59"/>
       <c r="E17" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="F17" s="46" t="s">
+      <c r="F17" s="37" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="49" customFormat="1" ht="71.25">
-      <c r="A18" s="46">
+    <row r="18" spans="1:6" s="38" customFormat="1" ht="71.25">
+      <c r="A18" s="37">
         <v>8</v>
       </c>
-      <c r="B18" s="47"/>
-      <c r="C18" s="47" t="s">
+      <c r="B18" s="43"/>
+      <c r="C18" s="43" t="s">
         <v>45</v>
       </c>
       <c r="D18" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="46" t="s">
+      <c r="E18" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="F18" s="46" t="s">
+      <c r="F18" s="37" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="49" customFormat="1" ht="71.25">
-      <c r="A19" s="46">
+    <row r="19" spans="1:6" s="38" customFormat="1" ht="71.25">
+      <c r="A19" s="37">
         <v>9</v>
       </c>
-      <c r="B19" s="47"/>
-      <c r="C19" s="47"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="43"/>
       <c r="D19" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="E19" s="46" t="s">
+      <c r="E19" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="F19" s="46" t="s">
+      <c r="F19" s="37" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="49" customFormat="1" ht="45">
-      <c r="A20" s="46">
+    <row r="20" spans="1:6" s="38" customFormat="1" ht="45">
+      <c r="A20" s="37">
         <v>10</v>
       </c>
-      <c r="B20" s="47"/>
-      <c r="C20" s="47" t="s">
+      <c r="B20" s="43"/>
+      <c r="C20" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="46" t="s">
+      <c r="D20" s="37" t="s">
         <v>43</v>
       </c>
       <c r="E20" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="F20" s="46" t="s">
+      <c r="F20" s="37" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="49" customFormat="1" ht="71.25">
-      <c r="A21" s="46">
+    <row r="21" spans="1:6" s="38" customFormat="1" ht="71.25">
+      <c r="A21" s="37">
         <v>11</v>
       </c>
-      <c r="B21" s="47"/>
-      <c r="C21" s="47"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="43"/>
       <c r="D21" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="E21" s="46" t="s">
+      <c r="E21" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="F21" s="46" t="s">
+      <c r="F21" s="37" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="49" customFormat="1" ht="71.25">
-      <c r="A22" s="46">
+    <row r="22" spans="1:6" s="38" customFormat="1" ht="71.25">
+      <c r="A22" s="37">
         <v>12</v>
       </c>
-      <c r="B22" s="47"/>
-      <c r="C22" s="47"/>
+      <c r="B22" s="43"/>
+      <c r="C22" s="43"/>
       <c r="D22" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="E22" s="46" t="s">
+      <c r="E22" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="F22" s="46" t="s">
+      <c r="F22" s="37" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="49" customFormat="1" ht="45">
-      <c r="A23" s="46">
+    <row r="23" spans="1:6" s="38" customFormat="1" ht="45">
+      <c r="A23" s="37">
         <v>13</v>
       </c>
-      <c r="B23" s="47"/>
-      <c r="C23" s="47" t="s">
+      <c r="B23" s="43"/>
+      <c r="C23" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="D23" s="46" t="s">
+      <c r="D23" s="37" t="s">
         <v>43</v>
       </c>
       <c r="E23" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="F23" s="46" t="s">
+      <c r="F23" s="37" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="49" customFormat="1" ht="71.25">
-      <c r="A24" s="46">
+    <row r="24" spans="1:6" s="38" customFormat="1" ht="71.25">
+      <c r="A24" s="37">
         <v>14</v>
       </c>
-      <c r="B24" s="47"/>
-      <c r="C24" s="47"/>
+      <c r="B24" s="43"/>
+      <c r="C24" s="43"/>
       <c r="D24" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="E24" s="46" t="s">
+      <c r="E24" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="F24" s="46" t="s">
+      <c r="F24" s="37" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="49" customFormat="1" ht="71.25">
-      <c r="A25" s="46">
+    <row r="25" spans="1:6" s="38" customFormat="1" ht="71.25">
+      <c r="A25" s="37">
         <v>15</v>
       </c>
-      <c r="B25" s="47"/>
-      <c r="C25" s="47"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="43"/>
       <c r="D25" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="E25" s="46" t="s">
+      <c r="E25" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="F25" s="46" t="s">
+      <c r="F25" s="37" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="53" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A26" s="53" t="s">
+    <row r="26" spans="1:6" s="56" customFormat="1" ht="23.25" customHeight="1">
+      <c r="A26" s="56" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="49" customFormat="1" ht="45">
-      <c r="A27" s="46">
+    <row r="27" spans="1:6" s="38" customFormat="1" ht="45">
+      <c r="A27" s="37">
         <v>15</v>
       </c>
-      <c r="B27" s="56" t="s">
+      <c r="B27" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="C27" s="47" t="s">
+      <c r="C27" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="D27" s="46" t="s">
+      <c r="D27" s="37" t="s">
         <v>43</v>
       </c>
       <c r="E27" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="F27" s="46" t="s">
+      <c r="F27" s="37" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="49" customFormat="1" ht="45">
-      <c r="A28" s="46">
+    <row r="28" spans="1:6" s="38" customFormat="1" ht="45">
+      <c r="A28" s="37">
         <v>16</v>
       </c>
-      <c r="B28" s="57"/>
-      <c r="C28" s="47"/>
-      <c r="D28" s="46" t="s">
+      <c r="B28" s="50"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="E28" s="46" t="s">
+      <c r="E28" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="F28" s="46" t="s">
+      <c r="F28" s="37" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="49" customFormat="1" ht="75">
-      <c r="A29" s="46">
+    <row r="29" spans="1:6" s="38" customFormat="1" ht="75">
+      <c r="A29" s="37">
         <v>17</v>
       </c>
-      <c r="B29" s="57"/>
-      <c r="C29" s="47"/>
-      <c r="D29" s="46" t="s">
+      <c r="B29" s="50"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="E29" s="46" t="s">
+      <c r="E29" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="F29" s="46" t="s">
+      <c r="F29" s="37" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="49" customFormat="1" ht="75">
-      <c r="A30" s="46">
+    <row r="30" spans="1:6" s="38" customFormat="1" ht="75">
+      <c r="A30" s="37">
         <v>18</v>
       </c>
-      <c r="B30" s="57"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="46" t="s">
+      <c r="B30" s="50"/>
+      <c r="C30" s="43"/>
+      <c r="D30" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="E30" s="46" t="s">
+      <c r="E30" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="F30" s="46" t="s">
+      <c r="F30" s="37" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="49" customFormat="1" ht="75">
-      <c r="A31" s="46">
+    <row r="31" spans="1:6" s="38" customFormat="1" ht="75">
+      <c r="A31" s="37">
         <v>19</v>
       </c>
-      <c r="B31" s="57"/>
-      <c r="C31" s="47"/>
-      <c r="D31" s="46" t="s">
+      <c r="B31" s="50"/>
+      <c r="C31" s="43"/>
+      <c r="D31" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="E31" s="46" t="s">
+      <c r="E31" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="F31" s="46" t="s">
+      <c r="F31" s="37" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="49" customFormat="1" ht="75">
-      <c r="A32" s="46">
+    <row r="32" spans="1:6" s="38" customFormat="1" ht="75">
+      <c r="A32" s="37">
         <v>20</v>
       </c>
-      <c r="B32" s="57"/>
-      <c r="C32" s="47"/>
-      <c r="D32" s="46" t="s">
+      <c r="B32" s="50"/>
+      <c r="C32" s="43"/>
+      <c r="D32" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="E32" s="46" t="s">
+      <c r="E32" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="F32" s="46" t="s">
+      <c r="F32" s="37" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="49" customFormat="1" ht="75">
-      <c r="A33" s="46">
+    <row r="33" spans="1:6" s="38" customFormat="1" ht="75">
+      <c r="A33" s="37">
         <v>21</v>
       </c>
-      <c r="B33" s="57"/>
-      <c r="C33" s="47"/>
-      <c r="D33" s="46" t="s">
+      <c r="B33" s="50"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="E33" s="46" t="s">
+      <c r="E33" s="37" t="s">
         <v>101</v>
       </c>
-      <c r="F33" s="46" t="s">
+      <c r="F33" s="37" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="49" customFormat="1" ht="45">
-      <c r="A34" s="46">
+    <row r="34" spans="1:6" s="38" customFormat="1" ht="45">
+      <c r="A34" s="37">
         <v>22</v>
       </c>
-      <c r="B34" s="57"/>
-      <c r="C34" s="47" t="s">
+      <c r="B34" s="50"/>
+      <c r="C34" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="D34" s="46" t="s">
+      <c r="D34" s="37" t="s">
         <v>43</v>
       </c>
       <c r="E34" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="F34" s="46" t="s">
+      <c r="F34" s="37" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="49" customFormat="1" ht="75">
-      <c r="A35" s="46">
+    <row r="35" spans="1:6" s="38" customFormat="1" ht="75">
+      <c r="A35" s="37">
         <v>23</v>
       </c>
-      <c r="B35" s="57"/>
-      <c r="C35" s="47"/>
-      <c r="D35" s="46" t="s">
+      <c r="B35" s="50"/>
+      <c r="C35" s="43"/>
+      <c r="D35" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="E35" s="46" t="s">
+      <c r="E35" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="F35" s="46" t="s">
+      <c r="F35" s="37" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="49" customFormat="1" ht="75">
-      <c r="A36" s="46">
+    <row r="36" spans="1:6" s="38" customFormat="1" ht="75">
+      <c r="A36" s="37">
         <v>24</v>
       </c>
-      <c r="B36" s="58"/>
-      <c r="C36" s="47"/>
-      <c r="D36" s="46" t="s">
+      <c r="B36" s="51"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="E36" s="46" t="s">
+      <c r="E36" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="F36" s="46" t="s">
+      <c r="F36" s="37" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="54" customFormat="1">
-      <c r="A37" s="54" t="s">
+    <row r="37" spans="1:6" s="58" customFormat="1">
+      <c r="A37" s="58" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="38" spans="1:6" s="49" customFormat="1" ht="105">
-      <c r="A38" s="46">
+    <row r="38" spans="1:6" s="38" customFormat="1" ht="105">
+      <c r="A38" s="37">
         <v>25</v>
       </c>
-      <c r="B38" s="47" t="s">
+      <c r="B38" s="43" t="s">
         <v>107</v>
       </c>
-      <c r="C38" s="47" t="s">
+      <c r="C38" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="D38" s="47"/>
-      <c r="E38" s="46" t="s">
+      <c r="D38" s="43"/>
+      <c r="E38" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="F38" s="46" t="s">
+      <c r="F38" s="37" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="49" customFormat="1" ht="60">
-      <c r="A39" s="46">
+    <row r="39" spans="1:6" s="38" customFormat="1" ht="60">
+      <c r="A39" s="37">
         <v>26</v>
       </c>
-      <c r="B39" s="47"/>
-      <c r="C39" s="47" t="s">
+      <c r="B39" s="43"/>
+      <c r="C39" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="D39" s="46" t="s">
+      <c r="D39" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="E39" s="46" t="s">
+      <c r="E39" s="37" t="s">
         <v>112</v>
       </c>
-      <c r="F39" s="46" t="s">
+      <c r="F39" s="37" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="49" customFormat="1" ht="60">
-      <c r="A40" s="46">
+    <row r="40" spans="1:6" s="38" customFormat="1" ht="60">
+      <c r="A40" s="37">
         <v>27</v>
       </c>
-      <c r="B40" s="47"/>
-      <c r="C40" s="47"/>
-      <c r="D40" s="46" t="s">
+      <c r="B40" s="43"/>
+      <c r="C40" s="43"/>
+      <c r="D40" s="37" t="s">
         <v>113</v>
       </c>
-      <c r="E40" s="46" t="s">
+      <c r="E40" s="37" t="s">
         <v>115</v>
       </c>
-      <c r="F40" s="46" t="s">
+      <c r="F40" s="37" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="1:6" s="49" customFormat="1" ht="60">
-      <c r="A41" s="46">
+    <row r="41" spans="1:6" s="38" customFormat="1" ht="60">
+      <c r="A41" s="37">
         <v>28</v>
       </c>
-      <c r="B41" s="47"/>
-      <c r="C41" s="47"/>
-      <c r="D41" s="46" t="s">
+      <c r="B41" s="43"/>
+      <c r="C41" s="43"/>
+      <c r="D41" s="37" t="s">
         <v>114</v>
       </c>
-      <c r="E41" s="46" t="s">
+      <c r="E41" s="37" t="s">
         <v>116</v>
       </c>
-      <c r="F41" s="46" t="s">
+      <c r="F41" s="37" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="49" customFormat="1" ht="75">
-      <c r="A42" s="46">
+    <row r="42" spans="1:6" s="38" customFormat="1" ht="75">
+      <c r="A42" s="37">
         <v>29</v>
       </c>
-      <c r="B42" s="47"/>
-      <c r="C42" s="47" t="s">
+      <c r="B42" s="43"/>
+      <c r="C42" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="D42" s="46" t="s">
+      <c r="D42" s="37" t="s">
         <v>121</v>
       </c>
-      <c r="E42" s="46" t="s">
+      <c r="E42" s="37" t="s">
         <v>122</v>
       </c>
-      <c r="F42" s="46" t="s">
+      <c r="F42" s="37" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="49" customFormat="1" ht="75">
-      <c r="A43" s="46">
+    <row r="43" spans="1:6" s="38" customFormat="1" ht="75">
+      <c r="A43" s="37">
         <v>30</v>
       </c>
-      <c r="B43" s="47"/>
-      <c r="C43" s="47"/>
-      <c r="D43" s="46" t="s">
+      <c r="B43" s="43"/>
+      <c r="C43" s="43"/>
+      <c r="D43" s="37" t="s">
         <v>123</v>
       </c>
-      <c r="E43" s="46" t="s">
+      <c r="E43" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="F43" s="46" t="s">
+      <c r="F43" s="37" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="49" customFormat="1" ht="75">
-      <c r="A44" s="46">
+    <row r="44" spans="1:6" s="38" customFormat="1" ht="75">
+      <c r="A44" s="37">
         <v>31</v>
       </c>
-      <c r="B44" s="47"/>
-      <c r="C44" s="47"/>
-      <c r="D44" s="46" t="s">
+      <c r="B44" s="43"/>
+      <c r="C44" s="43"/>
+      <c r="D44" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="E44" s="46" t="s">
+      <c r="E44" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="F44" s="46" t="s">
+      <c r="F44" s="37" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="45" spans="1:6" s="49" customFormat="1" ht="75">
-      <c r="A45" s="46">
+    <row r="45" spans="1:6" s="38" customFormat="1" ht="75">
+      <c r="A45" s="37">
         <v>32</v>
       </c>
-      <c r="B45" s="47"/>
-      <c r="C45" s="47" t="s">
+      <c r="B45" s="43"/>
+      <c r="C45" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="D45" s="46" t="s">
+      <c r="D45" s="37" t="s">
         <v>131</v>
       </c>
-      <c r="E45" s="46" t="s">
+      <c r="E45" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="F45" s="46" t="s">
+      <c r="F45" s="37" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="46" spans="1:6" s="49" customFormat="1" ht="75">
-      <c r="A46" s="46">
+    <row r="46" spans="1:6" s="38" customFormat="1" ht="75">
+      <c r="A46" s="37">
         <v>33</v>
       </c>
-      <c r="B46" s="47"/>
-      <c r="C46" s="47"/>
-      <c r="D46" s="46" t="s">
+      <c r="B46" s="43"/>
+      <c r="C46" s="43"/>
+      <c r="D46" s="37" t="s">
         <v>133</v>
       </c>
-      <c r="E46" s="46" t="s">
+      <c r="E46" s="37" t="s">
         <v>134</v>
       </c>
-      <c r="F46" s="46" t="s">
+      <c r="F46" s="37" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="47" spans="1:6" s="49" customFormat="1" ht="75">
-      <c r="A47" s="46">
+    <row r="47" spans="1:6" s="38" customFormat="1" ht="75">
+      <c r="A47" s="37">
         <v>34</v>
       </c>
-      <c r="B47" s="47"/>
-      <c r="C47" s="47"/>
-      <c r="D47" s="46" t="s">
+      <c r="B47" s="43"/>
+      <c r="C47" s="43"/>
+      <c r="D47" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="E47" s="46" t="s">
+      <c r="E47" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="F47" s="46" t="s">
+      <c r="F47" s="37" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="48" spans="1:6" s="49" customFormat="1" ht="75">
-      <c r="A48" s="46">
+    <row r="48" spans="1:6" s="38" customFormat="1" ht="75">
+      <c r="A48" s="37">
         <v>35</v>
       </c>
-      <c r="B48" s="47"/>
-      <c r="C48" s="47" t="s">
+      <c r="B48" s="43"/>
+      <c r="C48" s="43" t="s">
         <v>138</v>
       </c>
-      <c r="D48" s="46" t="s">
+      <c r="D48" s="37" t="s">
         <v>139</v>
       </c>
-      <c r="E48" s="46" t="s">
+      <c r="E48" s="37" t="s">
         <v>140</v>
       </c>
-      <c r="F48" s="46" t="s">
+      <c r="F48" s="37" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="49" spans="1:6" s="49" customFormat="1" ht="75">
-      <c r="A49" s="46">
+    <row r="49" spans="1:6" s="38" customFormat="1" ht="75">
+      <c r="A49" s="37">
         <v>36</v>
       </c>
-      <c r="B49" s="47"/>
-      <c r="C49" s="47"/>
-      <c r="D49" s="46" t="s">
+      <c r="B49" s="43"/>
+      <c r="C49" s="43"/>
+      <c r="D49" s="37" t="s">
         <v>141</v>
       </c>
-      <c r="E49" s="46" t="s">
+      <c r="E49" s="37" t="s">
         <v>142</v>
       </c>
-      <c r="F49" s="46" t="s">
+      <c r="F49" s="37" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="50" spans="1:6" s="49" customFormat="1" ht="75">
-      <c r="A50" s="46">
+    <row r="50" spans="1:6" s="38" customFormat="1" ht="75">
+      <c r="A50" s="37">
         <v>37</v>
       </c>
-      <c r="B50" s="47"/>
-      <c r="C50" s="47"/>
-      <c r="D50" s="46" t="s">
+      <c r="B50" s="43"/>
+      <c r="C50" s="43"/>
+      <c r="D50" s="37" t="s">
         <v>143</v>
       </c>
-      <c r="E50" s="46" t="s">
+      <c r="E50" s="37" t="s">
         <v>144</v>
       </c>
-      <c r="F50" s="46" t="s">
+      <c r="F50" s="37" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="51" spans="1:6" s="49" customFormat="1" ht="90">
-      <c r="A51" s="46">
+    <row r="51" spans="1:6" s="38" customFormat="1" ht="90">
+      <c r="A51" s="37">
         <v>38</v>
       </c>
-      <c r="B51" s="47"/>
-      <c r="C51" s="47" t="s">
+      <c r="B51" s="43"/>
+      <c r="C51" s="43" t="s">
         <v>146</v>
       </c>
-      <c r="D51" s="46" t="s">
+      <c r="D51" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="E51" s="46" t="s">
+      <c r="E51" s="37" t="s">
         <v>147</v>
       </c>
-      <c r="F51" s="46" t="s">
+      <c r="F51" s="37" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="52" spans="1:6" s="49" customFormat="1" ht="45">
-      <c r="A52" s="46">
+    <row r="52" spans="1:6" s="38" customFormat="1" ht="45">
+      <c r="A52" s="37">
         <v>39</v>
       </c>
-      <c r="B52" s="47"/>
-      <c r="C52" s="47"/>
-      <c r="D52" s="46" t="s">
+      <c r="B52" s="43"/>
+      <c r="C52" s="43"/>
+      <c r="D52" s="37" t="s">
         <v>149</v>
       </c>
-      <c r="E52" s="46" t="s">
+      <c r="E52" s="37" t="s">
         <v>148</v>
       </c>
-      <c r="F52" s="46" t="s">
+      <c r="F52" s="37" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="53" spans="1:6" s="49" customFormat="1" ht="45">
-      <c r="A53" s="46">
+    <row r="53" spans="1:6" s="38" customFormat="1" ht="45">
+      <c r="A53" s="37">
         <v>40</v>
       </c>
-      <c r="B53" s="47"/>
-      <c r="C53" s="47"/>
-      <c r="D53" s="46" t="s">
+      <c r="B53" s="43"/>
+      <c r="C53" s="43"/>
+      <c r="D53" s="37" t="s">
         <v>150</v>
       </c>
-      <c r="E53" s="46" t="s">
+      <c r="E53" s="37" t="s">
         <v>151</v>
       </c>
-      <c r="F53" s="46" t="s">
+      <c r="F53" s="37" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="54" spans="1:6" s="49" customFormat="1" ht="60">
-      <c r="A54" s="46">
+    <row r="54" spans="1:6" s="38" customFormat="1" ht="60">
+      <c r="A54" s="37">
         <v>41</v>
       </c>
-      <c r="B54" s="47"/>
-      <c r="C54" s="47"/>
-      <c r="D54" s="46" t="s">
+      <c r="B54" s="43"/>
+      <c r="C54" s="43"/>
+      <c r="D54" s="37" t="s">
         <v>153</v>
       </c>
-      <c r="E54" s="46" t="s">
+      <c r="E54" s="37" t="s">
         <v>154</v>
       </c>
-      <c r="F54" s="46" t="s">
+      <c r="F54" s="37" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="55" spans="1:6" s="49" customFormat="1" ht="45">
-      <c r="A55" s="46">
+    <row r="55" spans="1:6" s="38" customFormat="1" ht="45">
+      <c r="A55" s="37">
         <v>42</v>
       </c>
-      <c r="B55" s="47"/>
-      <c r="C55" s="47"/>
-      <c r="D55" s="46" t="s">
+      <c r="B55" s="43"/>
+      <c r="C55" s="43"/>
+      <c r="D55" s="37" t="s">
         <v>158</v>
       </c>
-      <c r="E55" s="46" t="s">
+      <c r="E55" s="37" t="s">
         <v>159</v>
       </c>
-      <c r="F55" s="46" t="s">
+      <c r="F55" s="37" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="56" spans="1:6" s="49" customFormat="1" ht="45">
-      <c r="A56" s="46">
+    <row r="56" spans="1:6" s="38" customFormat="1" ht="45">
+      <c r="A56" s="37">
         <v>43</v>
       </c>
-      <c r="B56" s="47"/>
-      <c r="C56" s="47" t="s">
+      <c r="B56" s="43"/>
+      <c r="C56" s="43" t="s">
         <v>157</v>
       </c>
-      <c r="D56" s="46" t="s">
+      <c r="D56" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="E56" s="46" t="s">
+      <c r="E56" s="37" t="s">
         <v>161</v>
       </c>
-      <c r="F56" s="46" t="s">
+      <c r="F56" s="37" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="57" spans="1:6" s="49" customFormat="1" ht="60">
-      <c r="A57" s="46">
+    <row r="57" spans="1:6" s="38" customFormat="1" ht="60">
+      <c r="A57" s="37">
         <v>44</v>
       </c>
-      <c r="B57" s="47"/>
-      <c r="C57" s="47"/>
-      <c r="D57" s="46" t="s">
+      <c r="B57" s="43"/>
+      <c r="C57" s="43"/>
+      <c r="D57" s="37" t="s">
         <v>162</v>
       </c>
-      <c r="E57" s="46" t="s">
+      <c r="E57" s="37" t="s">
         <v>163</v>
       </c>
-      <c r="F57" s="46" t="s">
+      <c r="F57" s="37" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="58" spans="1:6" s="49" customFormat="1" ht="60">
-      <c r="A58" s="46">
+    <row r="58" spans="1:6" s="38" customFormat="1" ht="60">
+      <c r="A58" s="37">
         <v>45</v>
       </c>
-      <c r="B58" s="47"/>
-      <c r="C58" s="47"/>
-      <c r="D58" s="46" t="s">
+      <c r="B58" s="43"/>
+      <c r="C58" s="43"/>
+      <c r="D58" s="37" t="s">
         <v>164</v>
       </c>
-      <c r="E58" s="46" t="s">
+      <c r="E58" s="37" t="s">
         <v>165</v>
       </c>
-      <c r="F58" s="46" t="s">
+      <c r="F58" s="37" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="59" spans="1:6" s="49" customFormat="1" ht="45">
-      <c r="A59" s="46">
+    <row r="59" spans="1:6" s="38" customFormat="1" ht="45">
+      <c r="A59" s="37">
         <v>46</v>
       </c>
-      <c r="B59" s="47"/>
-      <c r="C59" s="47" t="s">
+      <c r="B59" s="43"/>
+      <c r="C59" s="43" t="s">
         <v>168</v>
       </c>
-      <c r="D59" s="46" t="s">
+      <c r="D59" s="37" t="s">
         <v>169</v>
       </c>
-      <c r="E59" s="46" t="s">
+      <c r="E59" s="37" t="s">
         <v>171</v>
       </c>
-      <c r="F59" s="46" t="s">
+      <c r="F59" s="37" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="60" spans="1:6" s="49" customFormat="1" ht="45">
-      <c r="A60" s="46">
+    <row r="60" spans="1:6" s="38" customFormat="1" ht="45">
+      <c r="A60" s="37">
         <v>47</v>
       </c>
-      <c r="B60" s="47"/>
-      <c r="C60" s="47"/>
-      <c r="D60" s="46" t="s">
+      <c r="B60" s="43"/>
+      <c r="C60" s="43"/>
+      <c r="D60" s="37" t="s">
         <v>170</v>
       </c>
-      <c r="E60" s="46" t="s">
+      <c r="E60" s="37" t="s">
         <v>172</v>
       </c>
-      <c r="F60" s="46" t="s">
+      <c r="F60" s="37" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="61" spans="1:6" s="49" customFormat="1" ht="60">
-      <c r="A61" s="46">
+    <row r="61" spans="1:6" s="38" customFormat="1" ht="60">
+      <c r="A61" s="37">
         <v>48</v>
       </c>
-      <c r="B61" s="47"/>
-      <c r="C61" s="47" t="s">
+      <c r="B61" s="43"/>
+      <c r="C61" s="43" t="s">
         <v>174</v>
       </c>
-      <c r="D61" s="46" t="s">
+      <c r="D61" s="37" t="s">
         <v>175</v>
       </c>
-      <c r="E61" s="46" t="s">
+      <c r="E61" s="37" t="s">
         <v>176</v>
       </c>
-      <c r="F61" s="46" t="s">
+      <c r="F61" s="37" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="62" spans="1:6" s="49" customFormat="1" ht="60">
-      <c r="A62" s="46">
+    <row r="62" spans="1:6" s="38" customFormat="1" ht="60">
+      <c r="A62" s="37">
         <v>49</v>
       </c>
-      <c r="B62" s="47"/>
-      <c r="C62" s="47"/>
-      <c r="D62" s="46" t="s">
+      <c r="B62" s="43"/>
+      <c r="C62" s="43"/>
+      <c r="D62" s="37" t="s">
         <v>177</v>
       </c>
-      <c r="E62" s="46" t="s">
+      <c r="E62" s="37" t="s">
         <v>178</v>
       </c>
-      <c r="F62" s="46" t="s">
+      <c r="F62" s="37" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="63" spans="1:6" s="55" customFormat="1">
-      <c r="A63" s="55" t="s">
+    <row r="63" spans="1:6" s="48" customFormat="1">
+      <c r="A63" s="48" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="64" spans="1:6" s="49" customFormat="1" ht="45">
-      <c r="A64" s="46">
+    <row r="64" spans="1:6" s="38" customFormat="1" ht="45">
+      <c r="A64" s="37">
         <v>50</v>
       </c>
-      <c r="B64" s="46" t="s">
+      <c r="B64" s="37" t="s">
         <v>184</v>
       </c>
-      <c r="C64" s="47" t="s">
+      <c r="C64" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="D64" s="47"/>
-      <c r="E64" s="46" t="s">
+      <c r="D64" s="43"/>
+      <c r="E64" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="F64" s="46" t="s">
+      <c r="F64" s="37" t="s">
         <v>183</v>
       </c>
     </row>
@@ -2786,16 +3086,21 @@
     <mergeCell ref="C39:C41"/>
     <mergeCell ref="C42:C44"/>
     <mergeCell ref="C45:C47"/>
+    <mergeCell ref="A37:XFD37"/>
+    <mergeCell ref="B38:B62"/>
+    <mergeCell ref="C27:C33"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="B17:B25"/>
+    <mergeCell ref="C18:C19"/>
     <mergeCell ref="C48:C50"/>
     <mergeCell ref="C51:C55"/>
     <mergeCell ref="C56:C58"/>
     <mergeCell ref="C59:C60"/>
     <mergeCell ref="C61:C62"/>
-    <mergeCell ref="A37:XFD37"/>
-    <mergeCell ref="B38:B62"/>
-    <mergeCell ref="C27:C33"/>
-    <mergeCell ref="C34:C36"/>
-    <mergeCell ref="C38:D38"/>
     <mergeCell ref="C64:D64"/>
     <mergeCell ref="A63:XFD63"/>
     <mergeCell ref="B27:B36"/>
@@ -2821,12 +3126,7 @@
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="G8:M8"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="C23:C25"/>
     <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="B17:B25"/>
-    <mergeCell ref="C18:C19"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P1:P9 JL1:JL9 TH1:TH9 ADD1:ADD9 AMZ1:AMZ9 AWV1:AWV9 BGR1:BGR9 BQN1:BQN9 CAJ1:CAJ9 CKF1:CKF9 CUB1:CUB9 DDX1:DDX9 DNT1:DNT9 DXP1:DXP9 EHL1:EHL9 ERH1:ERH9 FBD1:FBD9 FKZ1:FKZ9 FUV1:FUV9 GER1:GER9 GON1:GON9 GYJ1:GYJ9 HIF1:HIF9 HSB1:HSB9 IBX1:IBX9 ILT1:ILT9 IVP1:IVP9 JFL1:JFL9 JPH1:JPH9 JZD1:JZD9 KIZ1:KIZ9 KSV1:KSV9 LCR1:LCR9 LMN1:LMN9 LWJ1:LWJ9 MGF1:MGF9 MQB1:MQB9 MZX1:MZX9 NJT1:NJT9 NTP1:NTP9 ODL1:ODL9 ONH1:ONH9 OXD1:OXD9 PGZ1:PGZ9 PQV1:PQV9 QAR1:QAR9 QKN1:QKN9 QUJ1:QUJ9 REF1:REF9 ROB1:ROB9 RXX1:RXX9 SHT1:SHT9 SRP1:SRP9 TBL1:TBL9 TLH1:TLH9 TVD1:TVD9 UEZ1:UEZ9 UOV1:UOV9 UYR1:UYR9 VIN1:VIN9 VSJ1:VSJ9 WCF1:WCF9 WMB1:WMB9 WVX1:WVX9">
@@ -2843,12 +3143,2687 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:Q265"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" customWidth="1"/>
+    <col min="6" max="6" width="26.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" s="6" customFormat="1">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="5"/>
+    </row>
+    <row r="2" spans="1:17" s="8" customFormat="1" ht="16.5" customHeight="1">
+      <c r="A2" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="52"/>
+      <c r="C2" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="Q2" s="9"/>
+    </row>
+    <row r="3" spans="1:17" s="8" customFormat="1" ht="16.5" customHeight="1">
+      <c r="A3" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="53" t="s">
+        <v>146</v>
+      </c>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="Q3" s="9"/>
+    </row>
+    <row r="4" spans="1:17" s="8" customFormat="1" ht="16.5" customHeight="1">
+      <c r="A4" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="53"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="Q4" s="9"/>
+    </row>
+    <row r="5" spans="1:17" s="8" customFormat="1">
+      <c r="A5" s="52" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="52"/>
+      <c r="C5" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="Q5" s="9"/>
+    </row>
+    <row r="6" spans="1:17" s="20" customFormat="1" ht="16.5" customHeight="1">
+      <c r="A6" s="52"/>
+      <c r="B6" s="52"/>
+      <c r="C6" s="15">
+        <f>COUNTIF(P10:P64,"OK")</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="16">
+        <f>COUNTIF(P10:P64, "NG")</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="17">
+        <f>COUNTIF(P10:P64, "N/A")</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="18">
+        <f>SUM(C6:E6)</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="Q6" s="21"/>
+    </row>
+    <row r="7" spans="1:17" s="6" customFormat="1">
+      <c r="A7" s="22"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="22"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="22"/>
+      <c r="Q7" s="28"/>
+    </row>
+    <row r="8" spans="1:17" s="6" customFormat="1" ht="21.75" customHeight="1">
+      <c r="A8" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="41"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="46"/>
+      <c r="M8" s="47"/>
+      <c r="N8" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="O8" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="P8" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q8" s="42" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" s="6" customFormat="1" ht="16.5" customHeight="1">
+      <c r="A9" s="41"/>
+      <c r="B9" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="41"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="K9" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="L9" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="M9" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="N9" s="41"/>
+      <c r="O9" s="41"/>
+      <c r="P9" s="41"/>
+      <c r="Q9" s="42"/>
+    </row>
+    <row r="10" spans="1:17" s="38" customFormat="1" ht="142.5">
+      <c r="A10" s="37">
+        <v>1</v>
+      </c>
+      <c r="B10" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="44"/>
+      <c r="E10" s="30" t="s">
+        <v>186</v>
+      </c>
+      <c r="F10" s="30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" s="38" customFormat="1" ht="114">
+      <c r="A11" s="37">
+        <v>2</v>
+      </c>
+      <c r="B11" s="43"/>
+      <c r="C11" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="44"/>
+      <c r="E11" s="31" t="s">
+        <v>187</v>
+      </c>
+      <c r="F11" s="37" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" s="38" customFormat="1" ht="42.75">
+      <c r="A12" s="37">
+        <v>3</v>
+      </c>
+      <c r="B12" s="43"/>
+      <c r="C12" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="44"/>
+      <c r="E12" s="32" t="s">
+        <v>188</v>
+      </c>
+      <c r="F12" s="40" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" s="38" customFormat="1" ht="42.75">
+      <c r="A13" s="37">
+        <v>4</v>
+      </c>
+      <c r="B13" s="43"/>
+      <c r="C13" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="44"/>
+      <c r="E13" s="32" t="s">
+        <v>189</v>
+      </c>
+      <c r="F13" s="32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" s="38" customFormat="1" ht="42.75">
+      <c r="A14" s="37">
+        <v>5</v>
+      </c>
+      <c r="B14" s="43"/>
+      <c r="C14" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="44"/>
+      <c r="E14" s="32" t="s">
+        <v>190</v>
+      </c>
+      <c r="F14" s="32" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" s="38" customFormat="1" ht="28.5">
+      <c r="A15" s="37">
+        <v>6</v>
+      </c>
+      <c r="B15" s="43"/>
+      <c r="C15" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="44"/>
+      <c r="E15" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="F15" s="40" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" s="60" customFormat="1">
+      <c r="A16" s="60" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="38" customFormat="1" ht="90">
+      <c r="A17" s="37">
+        <v>7</v>
+      </c>
+      <c r="B17" s="61" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="62" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="62"/>
+      <c r="E17" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="F17" s="37" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="38" customFormat="1" ht="57">
+      <c r="A18" s="37">
+        <v>8</v>
+      </c>
+      <c r="B18" s="61"/>
+      <c r="C18" s="43" t="s">
+        <v>195</v>
+      </c>
+      <c r="D18" s="37" t="s">
+        <v>196</v>
+      </c>
+      <c r="E18" s="32" t="s">
+        <v>202</v>
+      </c>
+      <c r="F18" s="37" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="38" customFormat="1" ht="60">
+      <c r="A19" s="37">
+        <v>9</v>
+      </c>
+      <c r="B19" s="61"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="32" t="s">
+        <v>197</v>
+      </c>
+      <c r="E19" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="F19" s="37" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="38" customFormat="1" ht="45">
+      <c r="A20" s="37">
+        <v>10</v>
+      </c>
+      <c r="B20" s="61"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="32" t="s">
+        <v>198</v>
+      </c>
+      <c r="E20" s="37" t="s">
+        <v>204</v>
+      </c>
+      <c r="F20" s="37" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="38" customFormat="1" ht="60">
+      <c r="A21" s="37">
+        <v>11</v>
+      </c>
+      <c r="B21" s="61"/>
+      <c r="C21" s="43" t="s">
+        <v>201</v>
+      </c>
+      <c r="D21" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="37" t="s">
+        <v>205</v>
+      </c>
+      <c r="F21" s="37" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="38" customFormat="1" ht="75">
+      <c r="A22" s="37">
+        <v>12</v>
+      </c>
+      <c r="B22" s="61"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="37" t="s">
+        <v>207</v>
+      </c>
+      <c r="F22" s="37" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="38" customFormat="1" ht="30">
+      <c r="A23" s="37">
+        <v>13</v>
+      </c>
+      <c r="B23" s="61"/>
+      <c r="C23" s="43" t="s">
+        <v>209</v>
+      </c>
+      <c r="D23" s="32" t="s">
+        <v>211</v>
+      </c>
+      <c r="E23" s="37" t="s">
+        <v>213</v>
+      </c>
+      <c r="F23" s="37" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="38" customFormat="1" ht="30">
+      <c r="A24" s="37">
+        <v>14</v>
+      </c>
+      <c r="B24" s="61"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="32" t="s">
+        <v>212</v>
+      </c>
+      <c r="E24" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="F24" s="37" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="38" customFormat="1" ht="57">
+      <c r="A25" s="37">
+        <v>15</v>
+      </c>
+      <c r="B25" s="61"/>
+      <c r="C25" s="43" t="s">
+        <v>215</v>
+      </c>
+      <c r="D25" s="37" t="s">
+        <v>216</v>
+      </c>
+      <c r="E25" s="32" t="s">
+        <v>221</v>
+      </c>
+      <c r="F25" s="37" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="38" customFormat="1" ht="60">
+      <c r="A26" s="37">
+        <v>16</v>
+      </c>
+      <c r="B26" s="61"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="E26" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="F26" s="37" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="38" customFormat="1" ht="60">
+      <c r="A27" s="37">
+        <v>17</v>
+      </c>
+      <c r="B27" s="61"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="32" t="s">
+        <v>218</v>
+      </c>
+      <c r="E27" s="37" t="s">
+        <v>220</v>
+      </c>
+      <c r="F27" s="37" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="38" customFormat="1" ht="57">
+      <c r="A28" s="37">
+        <v>18</v>
+      </c>
+      <c r="B28" s="61"/>
+      <c r="C28" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="F28" s="37" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="38" customFormat="1" ht="60">
+      <c r="A29" s="37">
+        <v>19</v>
+      </c>
+      <c r="B29" s="61"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" s="37" t="s">
+        <v>224</v>
+      </c>
+      <c r="F29" s="37" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="38" customFormat="1" ht="45">
+      <c r="A30" s="37">
+        <v>20</v>
+      </c>
+      <c r="B30" s="61"/>
+      <c r="C30" s="43"/>
+      <c r="D30" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="E30" s="37" t="s">
+        <v>225</v>
+      </c>
+      <c r="F30" s="37" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="38" customFormat="1" ht="57">
+      <c r="A31" s="37">
+        <v>21</v>
+      </c>
+      <c r="B31" s="61"/>
+      <c r="C31" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" s="32" t="s">
+        <v>226</v>
+      </c>
+      <c r="F31" s="37" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" s="38" customFormat="1" ht="60">
+      <c r="A32" s="37">
+        <v>22</v>
+      </c>
+      <c r="B32" s="61"/>
+      <c r="C32" s="43"/>
+      <c r="D32" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="E32" s="37" t="s">
+        <v>227</v>
+      </c>
+      <c r="F32" s="37" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" s="38" customFormat="1" ht="45">
+      <c r="A33" s="37">
+        <v>23</v>
+      </c>
+      <c r="B33" s="61"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="E33" s="37" t="s">
+        <v>228</v>
+      </c>
+      <c r="F33" s="37" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="58" customFormat="1">
+      <c r="A34" s="58" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="38" customFormat="1" ht="195">
+      <c r="A35" s="37">
+        <v>24</v>
+      </c>
+      <c r="B35" s="61" t="s">
+        <v>107</v>
+      </c>
+      <c r="C35" s="62" t="s">
+        <v>43</v>
+      </c>
+      <c r="D35" s="62"/>
+      <c r="E35" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="F35" s="37" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="38" customFormat="1" ht="75">
+      <c r="A36" s="37">
+        <v>25</v>
+      </c>
+      <c r="B36" s="61"/>
+      <c r="C36" s="37" t="s">
+        <v>230</v>
+      </c>
+      <c r="D36" s="37" t="s">
+        <v>231</v>
+      </c>
+      <c r="E36" s="37" t="s">
+        <v>232</v>
+      </c>
+      <c r="F36" s="37" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="38" customFormat="1" ht="45">
+      <c r="A37" s="37">
+        <v>26</v>
+      </c>
+      <c r="B37" s="61"/>
+      <c r="C37" s="43" t="s">
+        <v>234</v>
+      </c>
+      <c r="D37" s="32" t="s">
+        <v>235</v>
+      </c>
+      <c r="E37" s="37" t="s">
+        <v>237</v>
+      </c>
+      <c r="F37" s="37" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" s="38" customFormat="1" ht="30">
+      <c r="A38" s="37">
+        <v>27</v>
+      </c>
+      <c r="B38" s="61"/>
+      <c r="C38" s="43"/>
+      <c r="D38" s="32" t="s">
+        <v>236</v>
+      </c>
+      <c r="E38" s="37" t="s">
+        <v>238</v>
+      </c>
+      <c r="F38" s="37" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="38" customFormat="1" ht="57">
+      <c r="A39" s="37">
+        <v>28</v>
+      </c>
+      <c r="B39" s="61"/>
+      <c r="C39" s="43" t="s">
+        <v>195</v>
+      </c>
+      <c r="D39" s="37" t="s">
+        <v>196</v>
+      </c>
+      <c r="E39" s="32" t="s">
+        <v>202</v>
+      </c>
+      <c r="F39" s="37" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="38" customFormat="1" ht="60">
+      <c r="A40" s="37">
+        <v>29</v>
+      </c>
+      <c r="B40" s="61"/>
+      <c r="C40" s="43"/>
+      <c r="D40" s="32" t="s">
+        <v>197</v>
+      </c>
+      <c r="E40" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="F40" s="37" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" s="38" customFormat="1" ht="45">
+      <c r="A41" s="37">
+        <v>30</v>
+      </c>
+      <c r="B41" s="61"/>
+      <c r="C41" s="43"/>
+      <c r="D41" s="32" t="s">
+        <v>198</v>
+      </c>
+      <c r="E41" s="37" t="s">
+        <v>204</v>
+      </c>
+      <c r="F41" s="37" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" s="38" customFormat="1" ht="45">
+      <c r="A42" s="37">
+        <v>31</v>
+      </c>
+      <c r="B42" s="61"/>
+      <c r="C42" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="D42" s="32" t="s">
+        <v>242</v>
+      </c>
+      <c r="E42" s="37" t="s">
+        <v>243</v>
+      </c>
+      <c r="F42" s="37" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" s="38" customFormat="1" ht="71.25">
+      <c r="A43" s="37">
+        <v>32</v>
+      </c>
+      <c r="B43" s="61"/>
+      <c r="C43" s="43" t="s">
+        <v>245</v>
+      </c>
+      <c r="D43" s="37" t="s">
+        <v>246</v>
+      </c>
+      <c r="E43" s="32" t="s">
+        <v>249</v>
+      </c>
+      <c r="F43" s="37" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" s="38" customFormat="1" ht="60">
+      <c r="A44" s="37">
+        <v>33</v>
+      </c>
+      <c r="B44" s="61"/>
+      <c r="C44" s="43"/>
+      <c r="D44" s="32" t="s">
+        <v>248</v>
+      </c>
+      <c r="E44" s="37" t="s">
+        <v>250</v>
+      </c>
+      <c r="F44" s="37" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" s="38" customFormat="1" ht="57">
+      <c r="A45" s="37">
+        <v>34</v>
+      </c>
+      <c r="B45" s="61"/>
+      <c r="C45" s="43"/>
+      <c r="D45" s="32" t="s">
+        <v>247</v>
+      </c>
+      <c r="E45" s="37" t="s">
+        <v>251</v>
+      </c>
+      <c r="F45" s="37" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" s="38" customFormat="1" ht="71.25">
+      <c r="A46" s="37">
+        <v>35</v>
+      </c>
+      <c r="B46" s="61"/>
+      <c r="C46" s="43" t="s">
+        <v>245</v>
+      </c>
+      <c r="D46" s="37" t="s">
+        <v>246</v>
+      </c>
+      <c r="E46" s="32" t="s">
+        <v>249</v>
+      </c>
+      <c r="F46" s="37" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" s="38" customFormat="1" ht="75">
+      <c r="A47" s="37">
+        <v>36</v>
+      </c>
+      <c r="B47" s="61"/>
+      <c r="C47" s="43"/>
+      <c r="D47" s="32" t="s">
+        <v>248</v>
+      </c>
+      <c r="E47" s="37" t="s">
+        <v>250</v>
+      </c>
+      <c r="F47" s="37" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" s="38" customFormat="1" ht="57">
+      <c r="A48" s="37">
+        <v>37</v>
+      </c>
+      <c r="B48" s="61"/>
+      <c r="C48" s="43"/>
+      <c r="D48" s="32" t="s">
+        <v>247</v>
+      </c>
+      <c r="E48" s="37" t="s">
+        <v>251</v>
+      </c>
+      <c r="F48" s="37" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" s="38" customFormat="1" ht="105">
+      <c r="A49" s="37">
+        <v>38</v>
+      </c>
+      <c r="B49" s="61"/>
+      <c r="C49" s="37" t="s">
+        <v>256</v>
+      </c>
+      <c r="D49" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="E49" s="32" t="s">
+        <v>257</v>
+      </c>
+      <c r="F49" s="37" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" s="38" customFormat="1" ht="60">
+      <c r="A50" s="37">
+        <v>39</v>
+      </c>
+      <c r="B50" s="61"/>
+      <c r="C50" s="43" t="s">
+        <v>259</v>
+      </c>
+      <c r="D50" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="E50" s="37" t="s">
+        <v>161</v>
+      </c>
+      <c r="F50" s="37" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" s="38" customFormat="1" ht="45">
+      <c r="A51" s="37">
+        <v>40</v>
+      </c>
+      <c r="B51" s="61"/>
+      <c r="C51" s="43"/>
+      <c r="D51" s="37" t="s">
+        <v>162</v>
+      </c>
+      <c r="E51" s="37" t="s">
+        <v>163</v>
+      </c>
+      <c r="F51" s="37" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" s="38" customFormat="1" ht="45">
+      <c r="A52" s="37">
+        <v>41</v>
+      </c>
+      <c r="B52" s="61"/>
+      <c r="C52" s="43"/>
+      <c r="D52" s="37" t="s">
+        <v>164</v>
+      </c>
+      <c r="E52" s="37" t="s">
+        <v>165</v>
+      </c>
+      <c r="F52" s="37" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" s="48" customFormat="1">
+      <c r="A53" s="48" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" s="38" customFormat="1" ht="45">
+      <c r="A54" s="37">
+        <v>42</v>
+      </c>
+      <c r="B54" s="37" t="s">
+        <v>184</v>
+      </c>
+      <c r="C54" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="D54" s="43"/>
+      <c r="E54" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="F54" s="37" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="29"/>
+      <c r="B55" s="29"/>
+      <c r="C55" s="29"/>
+      <c r="D55" s="29"/>
+      <c r="E55" s="29"/>
+      <c r="F55" s="29"/>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="29"/>
+      <c r="B56" s="29"/>
+      <c r="C56" s="29"/>
+      <c r="D56" s="29"/>
+      <c r="E56" s="29"/>
+      <c r="F56" s="29"/>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" s="29"/>
+      <c r="B57" s="29"/>
+      <c r="C57" s="29"/>
+      <c r="D57" s="29"/>
+      <c r="E57" s="29"/>
+      <c r="F57" s="29"/>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" s="29"/>
+      <c r="B58" s="29"/>
+      <c r="C58" s="29"/>
+      <c r="D58" s="29"/>
+      <c r="E58" s="29"/>
+      <c r="F58" s="29"/>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" s="29"/>
+      <c r="B59" s="29"/>
+      <c r="C59" s="29"/>
+      <c r="D59" s="29"/>
+      <c r="E59" s="29"/>
+      <c r="F59" s="29"/>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" s="29"/>
+      <c r="B60" s="29"/>
+      <c r="C60" s="29"/>
+      <c r="D60" s="29"/>
+      <c r="E60" s="29"/>
+      <c r="F60" s="29"/>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" s="29"/>
+      <c r="B61" s="29"/>
+      <c r="C61" s="29"/>
+      <c r="D61" s="29"/>
+      <c r="E61" s="29"/>
+      <c r="F61" s="29"/>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" s="29"/>
+      <c r="B62" s="29"/>
+      <c r="C62" s="29"/>
+      <c r="D62" s="29"/>
+      <c r="E62" s="29"/>
+      <c r="F62" s="29"/>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" s="29"/>
+      <c r="B63" s="29"/>
+      <c r="C63" s="29"/>
+      <c r="D63" s="29"/>
+      <c r="E63" s="29"/>
+      <c r="F63" s="29"/>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" s="29"/>
+      <c r="B64" s="29"/>
+      <c r="C64" s="29"/>
+      <c r="D64" s="29"/>
+      <c r="E64" s="29"/>
+      <c r="F64" s="29"/>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" s="29"/>
+      <c r="B65" s="29"/>
+      <c r="C65" s="29"/>
+      <c r="D65" s="29"/>
+      <c r="E65" s="29"/>
+      <c r="F65" s="29"/>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" s="29"/>
+      <c r="B66" s="29"/>
+      <c r="C66" s="29"/>
+      <c r="D66" s="29"/>
+      <c r="E66" s="29"/>
+      <c r="F66" s="29"/>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" s="29"/>
+      <c r="B67" s="29"/>
+      <c r="C67" s="29"/>
+      <c r="D67" s="29"/>
+      <c r="E67" s="29"/>
+      <c r="F67" s="29"/>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" s="29"/>
+      <c r="B68" s="29"/>
+      <c r="C68" s="29"/>
+      <c r="D68" s="29"/>
+      <c r="E68" s="29"/>
+      <c r="F68" s="29"/>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" s="29"/>
+      <c r="B69" s="29"/>
+      <c r="C69" s="29"/>
+      <c r="D69" s="29"/>
+      <c r="E69" s="29"/>
+      <c r="F69" s="29"/>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" s="29"/>
+      <c r="B70" s="29"/>
+      <c r="C70" s="29"/>
+      <c r="D70" s="29"/>
+      <c r="E70" s="29"/>
+      <c r="F70" s="29"/>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" s="29"/>
+      <c r="B71" s="29"/>
+      <c r="C71" s="29"/>
+      <c r="D71" s="29"/>
+      <c r="E71" s="29"/>
+      <c r="F71" s="29"/>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" s="29"/>
+      <c r="B72" s="29"/>
+      <c r="C72" s="29"/>
+      <c r="D72" s="29"/>
+      <c r="E72" s="29"/>
+      <c r="F72" s="29"/>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" s="29"/>
+      <c r="B73" s="29"/>
+      <c r="C73" s="29"/>
+      <c r="D73" s="29"/>
+      <c r="E73" s="29"/>
+      <c r="F73" s="29"/>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" s="29"/>
+      <c r="B74" s="29"/>
+      <c r="C74" s="29"/>
+      <c r="D74" s="29"/>
+      <c r="E74" s="29"/>
+      <c r="F74" s="29"/>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75" s="29"/>
+      <c r="B75" s="29"/>
+      <c r="C75" s="29"/>
+      <c r="D75" s="29"/>
+      <c r="E75" s="29"/>
+      <c r="F75" s="29"/>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" s="29"/>
+      <c r="B76" s="29"/>
+      <c r="C76" s="29"/>
+      <c r="D76" s="29"/>
+      <c r="E76" s="29"/>
+      <c r="F76" s="29"/>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" s="29"/>
+      <c r="B77" s="29"/>
+      <c r="C77" s="29"/>
+      <c r="D77" s="29"/>
+      <c r="E77" s="29"/>
+      <c r="F77" s="29"/>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" s="29"/>
+      <c r="B78" s="29"/>
+      <c r="C78" s="29"/>
+      <c r="D78" s="29"/>
+      <c r="E78" s="29"/>
+      <c r="F78" s="29"/>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" s="29"/>
+      <c r="B79" s="29"/>
+      <c r="C79" s="29"/>
+      <c r="D79" s="29"/>
+      <c r="E79" s="29"/>
+      <c r="F79" s="29"/>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" s="29"/>
+      <c r="B80" s="29"/>
+      <c r="C80" s="29"/>
+      <c r="D80" s="29"/>
+      <c r="E80" s="29"/>
+      <c r="F80" s="29"/>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" s="29"/>
+      <c r="B81" s="29"/>
+      <c r="C81" s="29"/>
+      <c r="D81" s="29"/>
+      <c r="E81" s="29"/>
+      <c r="F81" s="29"/>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" s="29"/>
+      <c r="B82" s="29"/>
+      <c r="C82" s="29"/>
+      <c r="D82" s="29"/>
+      <c r="E82" s="29"/>
+      <c r="F82" s="29"/>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" s="29"/>
+      <c r="B83" s="29"/>
+      <c r="C83" s="29"/>
+      <c r="D83" s="29"/>
+      <c r="E83" s="29"/>
+      <c r="F83" s="29"/>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" s="29"/>
+      <c r="B84" s="29"/>
+      <c r="C84" s="29"/>
+      <c r="D84" s="29"/>
+      <c r="E84" s="29"/>
+      <c r="F84" s="29"/>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" s="29"/>
+      <c r="B85" s="29"/>
+      <c r="C85" s="29"/>
+      <c r="D85" s="29"/>
+      <c r="E85" s="29"/>
+      <c r="F85" s="29"/>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" s="29"/>
+      <c r="B86" s="29"/>
+      <c r="C86" s="29"/>
+      <c r="D86" s="29"/>
+      <c r="E86" s="29"/>
+      <c r="F86" s="29"/>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" s="29"/>
+      <c r="B87" s="29"/>
+      <c r="C87" s="29"/>
+      <c r="D87" s="29"/>
+      <c r="E87" s="29"/>
+      <c r="F87" s="29"/>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" s="29"/>
+      <c r="B88" s="29"/>
+      <c r="C88" s="29"/>
+      <c r="D88" s="29"/>
+      <c r="E88" s="29"/>
+      <c r="F88" s="29"/>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" s="29"/>
+      <c r="B89" s="29"/>
+      <c r="C89" s="29"/>
+      <c r="D89" s="29"/>
+      <c r="E89" s="29"/>
+      <c r="F89" s="29"/>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" s="29"/>
+      <c r="B90" s="29"/>
+      <c r="C90" s="29"/>
+      <c r="D90" s="29"/>
+      <c r="E90" s="29"/>
+      <c r="F90" s="29"/>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91" s="29"/>
+      <c r="B91" s="29"/>
+      <c r="C91" s="29"/>
+      <c r="D91" s="29"/>
+      <c r="E91" s="29"/>
+      <c r="F91" s="29"/>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92" s="29"/>
+      <c r="B92" s="29"/>
+      <c r="C92" s="29"/>
+      <c r="D92" s="29"/>
+      <c r="E92" s="29"/>
+      <c r="F92" s="29"/>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93" s="29"/>
+      <c r="B93" s="29"/>
+      <c r="C93" s="29"/>
+      <c r="D93" s="29"/>
+      <c r="E93" s="29"/>
+      <c r="F93" s="29"/>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94" s="29"/>
+      <c r="B94" s="29"/>
+      <c r="C94" s="29"/>
+      <c r="D94" s="29"/>
+      <c r="E94" s="29"/>
+      <c r="F94" s="29"/>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95" s="29"/>
+      <c r="B95" s="29"/>
+      <c r="C95" s="29"/>
+      <c r="D95" s="29"/>
+      <c r="E95" s="29"/>
+      <c r="F95" s="29"/>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="A96" s="29"/>
+      <c r="B96" s="29"/>
+      <c r="C96" s="29"/>
+      <c r="D96" s="29"/>
+      <c r="E96" s="29"/>
+      <c r="F96" s="29"/>
+    </row>
+    <row r="97" spans="1:6">
+      <c r="A97" s="29"/>
+      <c r="B97" s="29"/>
+      <c r="C97" s="29"/>
+      <c r="D97" s="29"/>
+      <c r="E97" s="29"/>
+      <c r="F97" s="29"/>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98" s="29"/>
+      <c r="B98" s="29"/>
+      <c r="C98" s="29"/>
+      <c r="D98" s="29"/>
+      <c r="E98" s="29"/>
+      <c r="F98" s="29"/>
+    </row>
+    <row r="99" spans="1:6">
+      <c r="A99" s="29"/>
+      <c r="B99" s="29"/>
+      <c r="C99" s="29"/>
+      <c r="D99" s="29"/>
+      <c r="E99" s="29"/>
+      <c r="F99" s="29"/>
+    </row>
+    <row r="100" spans="1:6">
+      <c r="A100" s="29"/>
+      <c r="B100" s="29"/>
+      <c r="C100" s="29"/>
+      <c r="D100" s="29"/>
+      <c r="E100" s="29"/>
+      <c r="F100" s="29"/>
+    </row>
+    <row r="101" spans="1:6">
+      <c r="A101" s="29"/>
+      <c r="B101" s="29"/>
+      <c r="C101" s="29"/>
+      <c r="D101" s="29"/>
+      <c r="E101" s="29"/>
+      <c r="F101" s="29"/>
+    </row>
+    <row r="102" spans="1:6">
+      <c r="A102" s="29"/>
+      <c r="B102" s="29"/>
+      <c r="C102" s="29"/>
+      <c r="D102" s="29"/>
+      <c r="E102" s="29"/>
+      <c r="F102" s="29"/>
+    </row>
+    <row r="103" spans="1:6">
+      <c r="A103" s="29"/>
+      <c r="B103" s="29"/>
+      <c r="C103" s="29"/>
+      <c r="D103" s="29"/>
+      <c r="E103" s="29"/>
+      <c r="F103" s="29"/>
+    </row>
+    <row r="104" spans="1:6">
+      <c r="A104" s="29"/>
+      <c r="B104" s="29"/>
+      <c r="C104" s="29"/>
+      <c r="D104" s="29"/>
+      <c r="E104" s="29"/>
+      <c r="F104" s="29"/>
+    </row>
+    <row r="105" spans="1:6">
+      <c r="A105" s="29"/>
+      <c r="B105" s="29"/>
+      <c r="C105" s="29"/>
+      <c r="D105" s="29"/>
+      <c r="E105" s="29"/>
+      <c r="F105" s="29"/>
+    </row>
+    <row r="106" spans="1:6">
+      <c r="A106" s="29"/>
+      <c r="B106" s="29"/>
+      <c r="C106" s="29"/>
+      <c r="D106" s="29"/>
+      <c r="E106" s="29"/>
+      <c r="F106" s="29"/>
+    </row>
+    <row r="107" spans="1:6">
+      <c r="A107" s="29"/>
+      <c r="B107" s="29"/>
+      <c r="C107" s="29"/>
+      <c r="D107" s="29"/>
+      <c r="E107" s="29"/>
+      <c r="F107" s="29"/>
+    </row>
+    <row r="108" spans="1:6">
+      <c r="A108" s="29"/>
+      <c r="B108" s="29"/>
+      <c r="C108" s="29"/>
+      <c r="D108" s="29"/>
+      <c r="E108" s="29"/>
+      <c r="F108" s="29"/>
+    </row>
+    <row r="109" spans="1:6">
+      <c r="A109" s="29"/>
+      <c r="B109" s="29"/>
+      <c r="C109" s="29"/>
+      <c r="D109" s="29"/>
+      <c r="E109" s="29"/>
+      <c r="F109" s="29"/>
+    </row>
+    <row r="110" spans="1:6">
+      <c r="A110" s="29"/>
+      <c r="B110" s="29"/>
+      <c r="C110" s="29"/>
+      <c r="D110" s="29"/>
+      <c r="E110" s="29"/>
+      <c r="F110" s="29"/>
+    </row>
+    <row r="111" spans="1:6">
+      <c r="A111" s="29"/>
+      <c r="B111" s="29"/>
+      <c r="C111" s="29"/>
+      <c r="D111" s="29"/>
+      <c r="E111" s="29"/>
+      <c r="F111" s="29"/>
+    </row>
+    <row r="112" spans="1:6">
+      <c r="A112" s="29"/>
+      <c r="B112" s="29"/>
+      <c r="C112" s="29"/>
+      <c r="D112" s="29"/>
+      <c r="E112" s="29"/>
+      <c r="F112" s="29"/>
+    </row>
+    <row r="113" spans="1:6">
+      <c r="A113" s="29"/>
+      <c r="B113" s="29"/>
+      <c r="C113" s="29"/>
+      <c r="D113" s="29"/>
+      <c r="E113" s="29"/>
+      <c r="F113" s="29"/>
+    </row>
+    <row r="114" spans="1:6">
+      <c r="A114" s="29"/>
+      <c r="B114" s="29"/>
+      <c r="C114" s="29"/>
+      <c r="D114" s="29"/>
+      <c r="E114" s="29"/>
+      <c r="F114" s="29"/>
+    </row>
+    <row r="115" spans="1:6">
+      <c r="A115" s="29"/>
+      <c r="B115" s="29"/>
+      <c r="C115" s="29"/>
+      <c r="D115" s="29"/>
+      <c r="E115" s="29"/>
+      <c r="F115" s="29"/>
+    </row>
+    <row r="116" spans="1:6">
+      <c r="A116" s="29"/>
+      <c r="B116" s="29"/>
+      <c r="C116" s="29"/>
+      <c r="D116" s="29"/>
+      <c r="E116" s="29"/>
+      <c r="F116" s="29"/>
+    </row>
+    <row r="117" spans="1:6">
+      <c r="A117" s="29"/>
+      <c r="B117" s="29"/>
+      <c r="C117" s="29"/>
+      <c r="D117" s="29"/>
+      <c r="E117" s="29"/>
+      <c r="F117" s="29"/>
+    </row>
+    <row r="118" spans="1:6">
+      <c r="A118" s="29"/>
+      <c r="B118" s="29"/>
+      <c r="C118" s="29"/>
+      <c r="D118" s="29"/>
+      <c r="E118" s="29"/>
+      <c r="F118" s="29"/>
+    </row>
+    <row r="119" spans="1:6">
+      <c r="A119" s="29"/>
+      <c r="B119" s="29"/>
+      <c r="C119" s="29"/>
+      <c r="D119" s="29"/>
+      <c r="E119" s="29"/>
+      <c r="F119" s="29"/>
+    </row>
+    <row r="120" spans="1:6">
+      <c r="A120" s="29"/>
+      <c r="B120" s="29"/>
+      <c r="C120" s="29"/>
+      <c r="D120" s="29"/>
+      <c r="E120" s="29"/>
+      <c r="F120" s="29"/>
+    </row>
+    <row r="121" spans="1:6">
+      <c r="A121" s="29"/>
+      <c r="B121" s="29"/>
+      <c r="C121" s="29"/>
+      <c r="D121" s="29"/>
+      <c r="E121" s="29"/>
+      <c r="F121" s="29"/>
+    </row>
+    <row r="122" spans="1:6">
+      <c r="A122" s="29"/>
+      <c r="B122" s="29"/>
+      <c r="C122" s="29"/>
+      <c r="D122" s="29"/>
+      <c r="E122" s="29"/>
+      <c r="F122" s="29"/>
+    </row>
+    <row r="123" spans="1:6">
+      <c r="A123" s="29"/>
+      <c r="B123" s="29"/>
+      <c r="C123" s="29"/>
+      <c r="D123" s="29"/>
+      <c r="E123" s="29"/>
+      <c r="F123" s="29"/>
+    </row>
+    <row r="124" spans="1:6">
+      <c r="A124" s="29"/>
+      <c r="B124" s="29"/>
+      <c r="C124" s="29"/>
+      <c r="D124" s="29"/>
+      <c r="E124" s="29"/>
+      <c r="F124" s="29"/>
+    </row>
+    <row r="125" spans="1:6">
+      <c r="A125" s="29"/>
+      <c r="B125" s="29"/>
+      <c r="C125" s="29"/>
+      <c r="D125" s="29"/>
+      <c r="E125" s="29"/>
+      <c r="F125" s="29"/>
+    </row>
+    <row r="126" spans="1:6">
+      <c r="A126" s="29"/>
+      <c r="B126" s="29"/>
+      <c r="C126" s="29"/>
+      <c r="D126" s="29"/>
+      <c r="E126" s="29"/>
+      <c r="F126" s="29"/>
+    </row>
+    <row r="127" spans="1:6">
+      <c r="A127" s="29"/>
+      <c r="B127" s="29"/>
+      <c r="C127" s="29"/>
+      <c r="D127" s="29"/>
+      <c r="E127" s="29"/>
+      <c r="F127" s="29"/>
+    </row>
+    <row r="128" spans="1:6">
+      <c r="A128" s="29"/>
+      <c r="B128" s="29"/>
+      <c r="C128" s="29"/>
+      <c r="D128" s="29"/>
+      <c r="E128" s="29"/>
+      <c r="F128" s="29"/>
+    </row>
+    <row r="129" spans="1:6">
+      <c r="A129" s="29"/>
+      <c r="B129" s="29"/>
+      <c r="C129" s="29"/>
+      <c r="D129" s="29"/>
+      <c r="E129" s="29"/>
+      <c r="F129" s="29"/>
+    </row>
+    <row r="130" spans="1:6">
+      <c r="A130" s="29"/>
+      <c r="B130" s="29"/>
+      <c r="C130" s="29"/>
+      <c r="D130" s="29"/>
+      <c r="E130" s="29"/>
+      <c r="F130" s="29"/>
+    </row>
+    <row r="131" spans="1:6">
+      <c r="A131" s="29"/>
+      <c r="B131" s="29"/>
+      <c r="C131" s="29"/>
+      <c r="D131" s="29"/>
+      <c r="E131" s="29"/>
+      <c r="F131" s="29"/>
+    </row>
+    <row r="132" spans="1:6">
+      <c r="A132" s="29"/>
+      <c r="B132" s="29"/>
+      <c r="C132" s="29"/>
+      <c r="D132" s="29"/>
+      <c r="E132" s="29"/>
+      <c r="F132" s="29"/>
+    </row>
+    <row r="133" spans="1:6">
+      <c r="A133" s="29"/>
+      <c r="B133" s="29"/>
+      <c r="C133" s="29"/>
+      <c r="D133" s="29"/>
+      <c r="E133" s="29"/>
+      <c r="F133" s="29"/>
+    </row>
+    <row r="134" spans="1:6">
+      <c r="A134" s="29"/>
+      <c r="B134" s="29"/>
+      <c r="C134" s="29"/>
+      <c r="D134" s="29"/>
+      <c r="E134" s="29"/>
+      <c r="F134" s="29"/>
+    </row>
+    <row r="135" spans="1:6">
+      <c r="A135" s="29"/>
+      <c r="B135" s="29"/>
+      <c r="C135" s="29"/>
+      <c r="D135" s="29"/>
+      <c r="E135" s="29"/>
+      <c r="F135" s="29"/>
+    </row>
+    <row r="136" spans="1:6">
+      <c r="A136" s="29"/>
+      <c r="B136" s="29"/>
+      <c r="C136" s="29"/>
+      <c r="D136" s="29"/>
+      <c r="E136" s="29"/>
+      <c r="F136" s="29"/>
+    </row>
+    <row r="137" spans="1:6">
+      <c r="A137" s="29"/>
+      <c r="B137" s="29"/>
+      <c r="C137" s="29"/>
+      <c r="D137" s="29"/>
+      <c r="E137" s="29"/>
+      <c r="F137" s="29"/>
+    </row>
+    <row r="138" spans="1:6">
+      <c r="A138" s="29"/>
+      <c r="B138" s="29"/>
+      <c r="C138" s="29"/>
+      <c r="D138" s="29"/>
+      <c r="E138" s="29"/>
+      <c r="F138" s="29"/>
+    </row>
+    <row r="139" spans="1:6">
+      <c r="A139" s="29"/>
+      <c r="B139" s="29"/>
+      <c r="C139" s="29"/>
+      <c r="D139" s="29"/>
+      <c r="E139" s="29"/>
+      <c r="F139" s="29"/>
+    </row>
+    <row r="140" spans="1:6">
+      <c r="A140" s="29"/>
+      <c r="B140" s="29"/>
+      <c r="C140" s="29"/>
+      <c r="D140" s="29"/>
+      <c r="E140" s="29"/>
+      <c r="F140" s="29"/>
+    </row>
+    <row r="141" spans="1:6">
+      <c r="A141" s="29"/>
+      <c r="B141" s="29"/>
+      <c r="C141" s="29"/>
+      <c r="D141" s="29"/>
+      <c r="E141" s="29"/>
+      <c r="F141" s="29"/>
+    </row>
+    <row r="142" spans="1:6">
+      <c r="A142" s="29"/>
+      <c r="B142" s="29"/>
+      <c r="C142" s="29"/>
+      <c r="D142" s="29"/>
+      <c r="E142" s="29"/>
+      <c r="F142" s="29"/>
+    </row>
+    <row r="143" spans="1:6">
+      <c r="A143" s="29"/>
+      <c r="B143" s="29"/>
+      <c r="C143" s="29"/>
+      <c r="D143" s="29"/>
+      <c r="E143" s="29"/>
+      <c r="F143" s="29"/>
+    </row>
+    <row r="144" spans="1:6">
+      <c r="A144" s="29"/>
+      <c r="B144" s="29"/>
+      <c r="C144" s="29"/>
+      <c r="D144" s="29"/>
+      <c r="E144" s="29"/>
+      <c r="F144" s="29"/>
+    </row>
+    <row r="145" spans="1:6">
+      <c r="A145" s="29"/>
+      <c r="B145" s="29"/>
+      <c r="C145" s="29"/>
+      <c r="D145" s="29"/>
+      <c r="E145" s="29"/>
+      <c r="F145" s="29"/>
+    </row>
+    <row r="146" spans="1:6">
+      <c r="A146" s="29"/>
+      <c r="B146" s="29"/>
+      <c r="C146" s="29"/>
+      <c r="D146" s="29"/>
+      <c r="E146" s="29"/>
+      <c r="F146" s="29"/>
+    </row>
+    <row r="147" spans="1:6">
+      <c r="A147" s="29"/>
+      <c r="B147" s="29"/>
+      <c r="C147" s="29"/>
+      <c r="D147" s="29"/>
+      <c r="E147" s="29"/>
+      <c r="F147" s="29"/>
+    </row>
+    <row r="148" spans="1:6">
+      <c r="A148" s="29"/>
+      <c r="B148" s="29"/>
+      <c r="C148" s="29"/>
+      <c r="D148" s="29"/>
+      <c r="E148" s="29"/>
+      <c r="F148" s="29"/>
+    </row>
+    <row r="149" spans="1:6">
+      <c r="A149" s="29"/>
+      <c r="B149" s="29"/>
+      <c r="C149" s="29"/>
+      <c r="D149" s="29"/>
+      <c r="E149" s="29"/>
+      <c r="F149" s="29"/>
+    </row>
+    <row r="150" spans="1:6">
+      <c r="A150" s="29"/>
+      <c r="B150" s="29"/>
+      <c r="C150" s="29"/>
+      <c r="D150" s="29"/>
+      <c r="E150" s="29"/>
+      <c r="F150" s="29"/>
+    </row>
+    <row r="151" spans="1:6">
+      <c r="A151" s="29"/>
+      <c r="B151" s="29"/>
+      <c r="C151" s="29"/>
+      <c r="D151" s="29"/>
+      <c r="E151" s="29"/>
+      <c r="F151" s="29"/>
+    </row>
+    <row r="152" spans="1:6">
+      <c r="A152" s="29"/>
+      <c r="B152" s="29"/>
+      <c r="C152" s="29"/>
+      <c r="D152" s="29"/>
+      <c r="E152" s="29"/>
+      <c r="F152" s="29"/>
+    </row>
+    <row r="153" spans="1:6">
+      <c r="A153" s="29"/>
+      <c r="B153" s="29"/>
+      <c r="C153" s="29"/>
+      <c r="D153" s="29"/>
+      <c r="E153" s="29"/>
+      <c r="F153" s="29"/>
+    </row>
+    <row r="154" spans="1:6">
+      <c r="A154" s="29"/>
+      <c r="B154" s="29"/>
+      <c r="C154" s="29"/>
+      <c r="D154" s="29"/>
+      <c r="E154" s="29"/>
+      <c r="F154" s="29"/>
+    </row>
+    <row r="155" spans="1:6">
+      <c r="A155" s="29"/>
+      <c r="B155" s="29"/>
+      <c r="C155" s="29"/>
+      <c r="D155" s="29"/>
+      <c r="E155" s="29"/>
+      <c r="F155" s="29"/>
+    </row>
+    <row r="156" spans="1:6">
+      <c r="A156" s="29"/>
+      <c r="B156" s="29"/>
+      <c r="C156" s="29"/>
+      <c r="D156" s="29"/>
+      <c r="E156" s="29"/>
+      <c r="F156" s="29"/>
+    </row>
+    <row r="157" spans="1:6">
+      <c r="A157" s="29"/>
+      <c r="B157" s="29"/>
+      <c r="C157" s="29"/>
+      <c r="D157" s="29"/>
+      <c r="E157" s="29"/>
+      <c r="F157" s="29"/>
+    </row>
+    <row r="158" spans="1:6">
+      <c r="A158" s="29"/>
+      <c r="B158" s="29"/>
+      <c r="C158" s="29"/>
+      <c r="D158" s="29"/>
+      <c r="E158" s="29"/>
+      <c r="F158" s="29"/>
+    </row>
+    <row r="159" spans="1:6">
+      <c r="A159" s="29"/>
+      <c r="B159" s="29"/>
+      <c r="C159" s="29"/>
+      <c r="D159" s="29"/>
+      <c r="E159" s="29"/>
+      <c r="F159" s="29"/>
+    </row>
+    <row r="160" spans="1:6">
+      <c r="A160" s="29"/>
+      <c r="B160" s="29"/>
+      <c r="C160" s="29"/>
+      <c r="D160" s="29"/>
+      <c r="E160" s="29"/>
+      <c r="F160" s="29"/>
+    </row>
+    <row r="161" spans="1:6">
+      <c r="A161" s="29"/>
+      <c r="B161" s="29"/>
+      <c r="C161" s="29"/>
+      <c r="D161" s="29"/>
+      <c r="E161" s="29"/>
+      <c r="F161" s="29"/>
+    </row>
+    <row r="162" spans="1:6">
+      <c r="A162" s="29"/>
+      <c r="B162" s="29"/>
+      <c r="C162" s="29"/>
+      <c r="D162" s="29"/>
+      <c r="E162" s="29"/>
+      <c r="F162" s="29"/>
+    </row>
+    <row r="163" spans="1:6">
+      <c r="A163" s="29"/>
+      <c r="B163" s="29"/>
+      <c r="C163" s="29"/>
+      <c r="D163" s="29"/>
+      <c r="E163" s="29"/>
+      <c r="F163" s="29"/>
+    </row>
+    <row r="164" spans="1:6">
+      <c r="A164" s="29"/>
+      <c r="B164" s="29"/>
+      <c r="C164" s="29"/>
+      <c r="D164" s="29"/>
+      <c r="E164" s="29"/>
+      <c r="F164" s="29"/>
+    </row>
+    <row r="165" spans="1:6">
+      <c r="A165" s="29"/>
+      <c r="B165" s="29"/>
+      <c r="C165" s="29"/>
+      <c r="D165" s="29"/>
+      <c r="E165" s="29"/>
+      <c r="F165" s="29"/>
+    </row>
+    <row r="166" spans="1:6">
+      <c r="A166" s="29"/>
+      <c r="B166" s="29"/>
+      <c r="C166" s="29"/>
+      <c r="D166" s="29"/>
+      <c r="E166" s="29"/>
+      <c r="F166" s="29"/>
+    </row>
+    <row r="167" spans="1:6">
+      <c r="A167" s="29"/>
+      <c r="B167" s="29"/>
+      <c r="C167" s="29"/>
+      <c r="D167" s="29"/>
+      <c r="E167" s="29"/>
+      <c r="F167" s="29"/>
+    </row>
+    <row r="168" spans="1:6">
+      <c r="A168" s="29"/>
+      <c r="B168" s="29"/>
+      <c r="C168" s="29"/>
+      <c r="D168" s="29"/>
+      <c r="E168" s="29"/>
+      <c r="F168" s="29"/>
+    </row>
+    <row r="169" spans="1:6">
+      <c r="A169" s="29"/>
+      <c r="B169" s="29"/>
+      <c r="C169" s="29"/>
+      <c r="D169" s="29"/>
+      <c r="E169" s="29"/>
+      <c r="F169" s="29"/>
+    </row>
+    <row r="170" spans="1:6">
+      <c r="A170" s="29"/>
+      <c r="B170" s="29"/>
+      <c r="C170" s="29"/>
+      <c r="D170" s="29"/>
+      <c r="E170" s="29"/>
+      <c r="F170" s="29"/>
+    </row>
+    <row r="171" spans="1:6">
+      <c r="A171" s="29"/>
+      <c r="B171" s="29"/>
+      <c r="C171" s="29"/>
+      <c r="D171" s="29"/>
+      <c r="E171" s="29"/>
+      <c r="F171" s="29"/>
+    </row>
+    <row r="172" spans="1:6">
+      <c r="A172" s="29"/>
+      <c r="B172" s="29"/>
+      <c r="C172" s="29"/>
+      <c r="D172" s="29"/>
+      <c r="E172" s="29"/>
+      <c r="F172" s="29"/>
+    </row>
+    <row r="173" spans="1:6">
+      <c r="A173" s="29"/>
+      <c r="B173" s="29"/>
+      <c r="C173" s="29"/>
+      <c r="D173" s="29"/>
+      <c r="E173" s="29"/>
+      <c r="F173" s="29"/>
+    </row>
+    <row r="174" spans="1:6">
+      <c r="A174" s="29"/>
+      <c r="B174" s="29"/>
+      <c r="C174" s="29"/>
+      <c r="D174" s="29"/>
+      <c r="E174" s="29"/>
+      <c r="F174" s="29"/>
+    </row>
+    <row r="175" spans="1:6">
+      <c r="A175" s="29"/>
+      <c r="B175" s="29"/>
+      <c r="C175" s="29"/>
+      <c r="D175" s="29"/>
+      <c r="E175" s="29"/>
+      <c r="F175" s="29"/>
+    </row>
+    <row r="176" spans="1:6">
+      <c r="A176" s="29"/>
+      <c r="B176" s="29"/>
+      <c r="C176" s="29"/>
+      <c r="D176" s="29"/>
+      <c r="E176" s="29"/>
+      <c r="F176" s="29"/>
+    </row>
+    <row r="177" spans="1:6">
+      <c r="A177" s="29"/>
+      <c r="B177" s="29"/>
+      <c r="C177" s="29"/>
+      <c r="D177" s="29"/>
+      <c r="E177" s="29"/>
+      <c r="F177" s="29"/>
+    </row>
+    <row r="178" spans="1:6">
+      <c r="A178" s="29"/>
+      <c r="B178" s="29"/>
+      <c r="C178" s="29"/>
+      <c r="D178" s="29"/>
+      <c r="E178" s="29"/>
+      <c r="F178" s="29"/>
+    </row>
+    <row r="179" spans="1:6">
+      <c r="A179" s="29"/>
+      <c r="B179" s="29"/>
+      <c r="C179" s="29"/>
+      <c r="D179" s="29"/>
+      <c r="E179" s="29"/>
+      <c r="F179" s="29"/>
+    </row>
+    <row r="180" spans="1:6">
+      <c r="A180" s="29"/>
+      <c r="B180" s="29"/>
+      <c r="C180" s="29"/>
+      <c r="D180" s="29"/>
+      <c r="E180" s="29"/>
+      <c r="F180" s="29"/>
+    </row>
+    <row r="181" spans="1:6">
+      <c r="A181" s="29"/>
+      <c r="B181" s="29"/>
+      <c r="C181" s="29"/>
+      <c r="D181" s="29"/>
+      <c r="E181" s="29"/>
+      <c r="F181" s="29"/>
+    </row>
+    <row r="182" spans="1:6">
+      <c r="A182" s="29"/>
+      <c r="B182" s="29"/>
+      <c r="C182" s="29"/>
+      <c r="D182" s="29"/>
+      <c r="E182" s="29"/>
+      <c r="F182" s="29"/>
+    </row>
+    <row r="183" spans="1:6">
+      <c r="A183" s="29"/>
+      <c r="B183" s="29"/>
+      <c r="C183" s="29"/>
+      <c r="D183" s="29"/>
+      <c r="E183" s="29"/>
+      <c r="F183" s="29"/>
+    </row>
+    <row r="184" spans="1:6">
+      <c r="A184" s="29"/>
+      <c r="B184" s="29"/>
+      <c r="C184" s="29"/>
+      <c r="D184" s="29"/>
+      <c r="E184" s="29"/>
+      <c r="F184" s="29"/>
+    </row>
+    <row r="185" spans="1:6">
+      <c r="A185" s="29"/>
+      <c r="B185" s="29"/>
+      <c r="C185" s="29"/>
+      <c r="D185" s="29"/>
+      <c r="E185" s="29"/>
+      <c r="F185" s="29"/>
+    </row>
+    <row r="186" spans="1:6">
+      <c r="A186" s="29"/>
+      <c r="B186" s="29"/>
+      <c r="C186" s="29"/>
+      <c r="D186" s="29"/>
+      <c r="E186" s="29"/>
+      <c r="F186" s="29"/>
+    </row>
+    <row r="187" spans="1:6">
+      <c r="A187" s="29"/>
+      <c r="B187" s="29"/>
+      <c r="C187" s="29"/>
+      <c r="D187" s="29"/>
+      <c r="E187" s="29"/>
+      <c r="F187" s="29"/>
+    </row>
+    <row r="188" spans="1:6">
+      <c r="A188" s="29"/>
+      <c r="B188" s="29"/>
+      <c r="C188" s="29"/>
+      <c r="D188" s="29"/>
+      <c r="E188" s="29"/>
+      <c r="F188" s="29"/>
+    </row>
+    <row r="189" spans="1:6">
+      <c r="A189" s="29"/>
+      <c r="B189" s="29"/>
+      <c r="C189" s="29"/>
+      <c r="D189" s="29"/>
+      <c r="E189" s="29"/>
+      <c r="F189" s="29"/>
+    </row>
+    <row r="190" spans="1:6">
+      <c r="A190" s="29"/>
+      <c r="B190" s="29"/>
+      <c r="C190" s="29"/>
+      <c r="D190" s="29"/>
+      <c r="E190" s="29"/>
+      <c r="F190" s="29"/>
+    </row>
+    <row r="191" spans="1:6">
+      <c r="A191" s="29"/>
+      <c r="B191" s="29"/>
+      <c r="C191" s="29"/>
+      <c r="D191" s="29"/>
+      <c r="E191" s="29"/>
+      <c r="F191" s="29"/>
+    </row>
+    <row r="192" spans="1:6">
+      <c r="A192" s="29"/>
+      <c r="B192" s="29"/>
+      <c r="C192" s="29"/>
+      <c r="D192" s="29"/>
+      <c r="E192" s="29"/>
+      <c r="F192" s="29"/>
+    </row>
+    <row r="193" spans="1:6">
+      <c r="A193" s="29"/>
+      <c r="B193" s="29"/>
+      <c r="C193" s="29"/>
+      <c r="D193" s="29"/>
+      <c r="E193" s="29"/>
+      <c r="F193" s="29"/>
+    </row>
+    <row r="194" spans="1:6">
+      <c r="A194" s="29"/>
+      <c r="B194" s="29"/>
+      <c r="C194" s="29"/>
+      <c r="D194" s="29"/>
+      <c r="E194" s="29"/>
+      <c r="F194" s="29"/>
+    </row>
+    <row r="195" spans="1:6">
+      <c r="A195" s="29"/>
+      <c r="B195" s="29"/>
+      <c r="C195" s="29"/>
+      <c r="D195" s="29"/>
+      <c r="E195" s="29"/>
+      <c r="F195" s="29"/>
+    </row>
+    <row r="196" spans="1:6">
+      <c r="A196" s="29"/>
+      <c r="B196" s="29"/>
+      <c r="C196" s="29"/>
+      <c r="D196" s="29"/>
+      <c r="E196" s="29"/>
+      <c r="F196" s="29"/>
+    </row>
+    <row r="197" spans="1:6">
+      <c r="A197" s="29"/>
+      <c r="B197" s="29"/>
+      <c r="C197" s="29"/>
+      <c r="D197" s="29"/>
+      <c r="E197" s="29"/>
+      <c r="F197" s="29"/>
+    </row>
+    <row r="198" spans="1:6">
+      <c r="A198" s="29"/>
+      <c r="B198" s="29"/>
+      <c r="C198" s="29"/>
+      <c r="D198" s="29"/>
+      <c r="E198" s="29"/>
+      <c r="F198" s="29"/>
+    </row>
+    <row r="199" spans="1:6">
+      <c r="A199" s="29"/>
+      <c r="B199" s="29"/>
+      <c r="C199" s="29"/>
+      <c r="D199" s="29"/>
+      <c r="E199" s="29"/>
+      <c r="F199" s="29"/>
+    </row>
+    <row r="200" spans="1:6">
+      <c r="A200" s="29"/>
+      <c r="B200" s="29"/>
+      <c r="C200" s="29"/>
+      <c r="D200" s="29"/>
+      <c r="E200" s="29"/>
+      <c r="F200" s="29"/>
+    </row>
+    <row r="201" spans="1:6">
+      <c r="A201" s="29"/>
+      <c r="B201" s="29"/>
+      <c r="C201" s="29"/>
+      <c r="D201" s="29"/>
+      <c r="E201" s="29"/>
+      <c r="F201" s="29"/>
+    </row>
+    <row r="202" spans="1:6">
+      <c r="A202" s="29"/>
+      <c r="B202" s="29"/>
+      <c r="C202" s="29"/>
+      <c r="D202" s="29"/>
+      <c r="E202" s="29"/>
+      <c r="F202" s="29"/>
+    </row>
+    <row r="203" spans="1:6">
+      <c r="A203" s="29"/>
+      <c r="B203" s="29"/>
+      <c r="C203" s="29"/>
+      <c r="D203" s="29"/>
+      <c r="E203" s="29"/>
+      <c r="F203" s="29"/>
+    </row>
+    <row r="204" spans="1:6">
+      <c r="A204" s="29"/>
+      <c r="B204" s="29"/>
+      <c r="C204" s="29"/>
+      <c r="D204" s="29"/>
+      <c r="E204" s="29"/>
+      <c r="F204" s="29"/>
+    </row>
+    <row r="205" spans="1:6">
+      <c r="A205" s="29"/>
+      <c r="B205" s="29"/>
+      <c r="C205" s="29"/>
+      <c r="D205" s="29"/>
+      <c r="E205" s="29"/>
+      <c r="F205" s="29"/>
+    </row>
+    <row r="206" spans="1:6">
+      <c r="A206" s="29"/>
+      <c r="B206" s="29"/>
+      <c r="C206" s="29"/>
+      <c r="D206" s="29"/>
+      <c r="E206" s="29"/>
+      <c r="F206" s="29"/>
+    </row>
+    <row r="207" spans="1:6">
+      <c r="A207" s="29"/>
+      <c r="B207" s="29"/>
+      <c r="C207" s="29"/>
+      <c r="D207" s="29"/>
+      <c r="E207" s="29"/>
+      <c r="F207" s="29"/>
+    </row>
+    <row r="208" spans="1:6">
+      <c r="A208" s="29"/>
+      <c r="B208" s="29"/>
+      <c r="C208" s="29"/>
+      <c r="D208" s="29"/>
+      <c r="E208" s="29"/>
+      <c r="F208" s="29"/>
+    </row>
+    <row r="209" spans="1:6">
+      <c r="A209" s="29"/>
+      <c r="B209" s="29"/>
+      <c r="C209" s="29"/>
+      <c r="D209" s="29"/>
+      <c r="E209" s="29"/>
+      <c r="F209" s="29"/>
+    </row>
+    <row r="210" spans="1:6">
+      <c r="A210" s="29"/>
+      <c r="B210" s="29"/>
+      <c r="C210" s="29"/>
+      <c r="D210" s="29"/>
+      <c r="E210" s="29"/>
+      <c r="F210" s="29"/>
+    </row>
+    <row r="211" spans="1:6">
+      <c r="A211" s="29"/>
+      <c r="B211" s="29"/>
+      <c r="C211" s="29"/>
+      <c r="D211" s="29"/>
+      <c r="E211" s="29"/>
+      <c r="F211" s="29"/>
+    </row>
+    <row r="212" spans="1:6">
+      <c r="A212" s="29"/>
+      <c r="B212" s="29"/>
+      <c r="C212" s="29"/>
+      <c r="D212" s="29"/>
+      <c r="E212" s="29"/>
+      <c r="F212" s="29"/>
+    </row>
+    <row r="213" spans="1:6">
+      <c r="A213" s="29"/>
+      <c r="B213" s="29"/>
+      <c r="C213" s="29"/>
+      <c r="D213" s="29"/>
+      <c r="E213" s="29"/>
+      <c r="F213" s="29"/>
+    </row>
+    <row r="214" spans="1:6">
+      <c r="A214" s="29"/>
+      <c r="B214" s="29"/>
+      <c r="C214" s="29"/>
+      <c r="D214" s="29"/>
+      <c r="E214" s="29"/>
+      <c r="F214" s="29"/>
+    </row>
+    <row r="215" spans="1:6">
+      <c r="A215" s="29"/>
+      <c r="B215" s="29"/>
+      <c r="C215" s="29"/>
+      <c r="D215" s="29"/>
+      <c r="E215" s="29"/>
+      <c r="F215" s="29"/>
+    </row>
+    <row r="216" spans="1:6">
+      <c r="A216" s="29"/>
+      <c r="B216" s="29"/>
+      <c r="C216" s="29"/>
+      <c r="D216" s="29"/>
+      <c r="E216" s="29"/>
+      <c r="F216" s="29"/>
+    </row>
+    <row r="217" spans="1:6">
+      <c r="A217" s="29"/>
+      <c r="B217" s="29"/>
+      <c r="C217" s="29"/>
+      <c r="D217" s="29"/>
+      <c r="E217" s="29"/>
+      <c r="F217" s="29"/>
+    </row>
+    <row r="218" spans="1:6">
+      <c r="A218" s="29"/>
+      <c r="B218" s="29"/>
+      <c r="C218" s="29"/>
+      <c r="D218" s="29"/>
+      <c r="E218" s="29"/>
+      <c r="F218" s="29"/>
+    </row>
+    <row r="219" spans="1:6">
+      <c r="A219" s="29"/>
+      <c r="B219" s="29"/>
+      <c r="C219" s="29"/>
+      <c r="D219" s="29"/>
+      <c r="E219" s="29"/>
+      <c r="F219" s="29"/>
+    </row>
+    <row r="220" spans="1:6">
+      <c r="A220" s="29"/>
+      <c r="B220" s="29"/>
+      <c r="C220" s="29"/>
+      <c r="D220" s="29"/>
+      <c r="E220" s="29"/>
+      <c r="F220" s="29"/>
+    </row>
+    <row r="221" spans="1:6">
+      <c r="A221" s="29"/>
+      <c r="B221" s="29"/>
+      <c r="C221" s="29"/>
+      <c r="D221" s="29"/>
+      <c r="E221" s="29"/>
+      <c r="F221" s="29"/>
+    </row>
+    <row r="222" spans="1:6">
+      <c r="A222" s="29"/>
+      <c r="B222" s="29"/>
+      <c r="C222" s="29"/>
+      <c r="D222" s="29"/>
+      <c r="E222" s="29"/>
+      <c r="F222" s="29"/>
+    </row>
+    <row r="223" spans="1:6">
+      <c r="A223" s="29"/>
+      <c r="B223" s="29"/>
+      <c r="C223" s="29"/>
+      <c r="D223" s="29"/>
+      <c r="E223" s="29"/>
+      <c r="F223" s="29"/>
+    </row>
+    <row r="224" spans="1:6">
+      <c r="A224" s="29"/>
+      <c r="B224" s="29"/>
+      <c r="C224" s="29"/>
+      <c r="D224" s="29"/>
+      <c r="E224" s="29"/>
+      <c r="F224" s="29"/>
+    </row>
+    <row r="225" spans="1:6">
+      <c r="A225" s="29"/>
+      <c r="B225" s="29"/>
+      <c r="C225" s="29"/>
+      <c r="D225" s="29"/>
+      <c r="E225" s="29"/>
+      <c r="F225" s="29"/>
+    </row>
+    <row r="226" spans="1:6">
+      <c r="A226" s="29"/>
+      <c r="B226" s="29"/>
+      <c r="C226" s="29"/>
+      <c r="D226" s="29"/>
+      <c r="E226" s="29"/>
+      <c r="F226" s="29"/>
+    </row>
+    <row r="227" spans="1:6">
+      <c r="A227" s="29"/>
+      <c r="B227" s="29"/>
+      <c r="C227" s="29"/>
+      <c r="D227" s="29"/>
+      <c r="E227" s="29"/>
+      <c r="F227" s="29"/>
+    </row>
+    <row r="228" spans="1:6">
+      <c r="A228" s="29"/>
+      <c r="B228" s="29"/>
+      <c r="C228" s="29"/>
+      <c r="D228" s="29"/>
+      <c r="E228" s="29"/>
+      <c r="F228" s="29"/>
+    </row>
+    <row r="229" spans="1:6">
+      <c r="A229" s="29"/>
+      <c r="B229" s="29"/>
+      <c r="C229" s="29"/>
+      <c r="D229" s="29"/>
+      <c r="E229" s="29"/>
+      <c r="F229" s="29"/>
+    </row>
+    <row r="230" spans="1:6">
+      <c r="A230" s="29"/>
+      <c r="B230" s="29"/>
+      <c r="C230" s="29"/>
+      <c r="D230" s="29"/>
+      <c r="E230" s="29"/>
+      <c r="F230" s="29"/>
+    </row>
+    <row r="231" spans="1:6">
+      <c r="A231" s="29"/>
+      <c r="B231" s="29"/>
+      <c r="C231" s="29"/>
+      <c r="D231" s="29"/>
+      <c r="E231" s="29"/>
+      <c r="F231" s="29"/>
+    </row>
+    <row r="232" spans="1:6">
+      <c r="A232" s="29"/>
+      <c r="B232" s="29"/>
+      <c r="C232" s="29"/>
+      <c r="D232" s="29"/>
+      <c r="E232" s="29"/>
+      <c r="F232" s="29"/>
+    </row>
+    <row r="233" spans="1:6">
+      <c r="A233" s="29"/>
+      <c r="B233" s="29"/>
+      <c r="C233" s="29"/>
+      <c r="D233" s="29"/>
+      <c r="E233" s="29"/>
+      <c r="F233" s="29"/>
+    </row>
+    <row r="234" spans="1:6">
+      <c r="A234" s="29"/>
+      <c r="B234" s="29"/>
+      <c r="C234" s="29"/>
+      <c r="D234" s="29"/>
+      <c r="E234" s="29"/>
+      <c r="F234" s="29"/>
+    </row>
+    <row r="235" spans="1:6">
+      <c r="A235" s="29"/>
+      <c r="B235" s="29"/>
+      <c r="C235" s="29"/>
+      <c r="D235" s="29"/>
+      <c r="E235" s="29"/>
+      <c r="F235" s="29"/>
+    </row>
+    <row r="236" spans="1:6">
+      <c r="A236" s="29"/>
+      <c r="B236" s="29"/>
+      <c r="C236" s="29"/>
+      <c r="D236" s="29"/>
+      <c r="E236" s="29"/>
+      <c r="F236" s="29"/>
+    </row>
+    <row r="237" spans="1:6">
+      <c r="A237" s="29"/>
+      <c r="B237" s="29"/>
+      <c r="C237" s="29"/>
+      <c r="D237" s="29"/>
+      <c r="E237" s="29"/>
+      <c r="F237" s="29"/>
+    </row>
+    <row r="238" spans="1:6">
+      <c r="A238" s="29"/>
+      <c r="B238" s="29"/>
+      <c r="C238" s="29"/>
+      <c r="D238" s="29"/>
+      <c r="E238" s="29"/>
+      <c r="F238" s="29"/>
+    </row>
+    <row r="239" spans="1:6">
+      <c r="A239" s="29"/>
+      <c r="B239" s="29"/>
+      <c r="C239" s="29"/>
+      <c r="D239" s="29"/>
+      <c r="E239" s="29"/>
+      <c r="F239" s="29"/>
+    </row>
+    <row r="240" spans="1:6">
+      <c r="A240" s="29"/>
+      <c r="B240" s="29"/>
+      <c r="C240" s="29"/>
+      <c r="D240" s="29"/>
+      <c r="E240" s="29"/>
+      <c r="F240" s="29"/>
+    </row>
+    <row r="241" spans="1:6">
+      <c r="A241" s="29"/>
+      <c r="B241" s="29"/>
+      <c r="C241" s="29"/>
+      <c r="D241" s="29"/>
+      <c r="E241" s="29"/>
+      <c r="F241" s="29"/>
+    </row>
+    <row r="242" spans="1:6">
+      <c r="A242" s="29"/>
+      <c r="B242" s="29"/>
+      <c r="C242" s="29"/>
+      <c r="D242" s="29"/>
+      <c r="E242" s="29"/>
+      <c r="F242" s="29"/>
+    </row>
+    <row r="243" spans="1:6">
+      <c r="A243" s="29"/>
+      <c r="B243" s="29"/>
+      <c r="C243" s="29"/>
+      <c r="D243" s="29"/>
+      <c r="E243" s="29"/>
+      <c r="F243" s="29"/>
+    </row>
+    <row r="244" spans="1:6">
+      <c r="A244" s="29"/>
+      <c r="B244" s="29"/>
+      <c r="C244" s="29"/>
+      <c r="D244" s="29"/>
+      <c r="E244" s="29"/>
+      <c r="F244" s="29"/>
+    </row>
+    <row r="245" spans="1:6">
+      <c r="A245" s="29"/>
+      <c r="B245" s="29"/>
+      <c r="C245" s="29"/>
+      <c r="D245" s="29"/>
+      <c r="E245" s="29"/>
+      <c r="F245" s="29"/>
+    </row>
+    <row r="246" spans="1:6">
+      <c r="A246" s="29"/>
+      <c r="B246" s="29"/>
+      <c r="C246" s="29"/>
+      <c r="D246" s="29"/>
+      <c r="E246" s="29"/>
+      <c r="F246" s="29"/>
+    </row>
+    <row r="247" spans="1:6">
+      <c r="A247" s="29"/>
+      <c r="B247" s="29"/>
+      <c r="C247" s="29"/>
+      <c r="D247" s="29"/>
+      <c r="E247" s="29"/>
+      <c r="F247" s="29"/>
+    </row>
+    <row r="248" spans="1:6">
+      <c r="A248" s="29"/>
+      <c r="B248" s="29"/>
+      <c r="C248" s="29"/>
+      <c r="D248" s="29"/>
+      <c r="E248" s="29"/>
+      <c r="F248" s="29"/>
+    </row>
+    <row r="249" spans="1:6">
+      <c r="A249" s="29"/>
+      <c r="B249" s="29"/>
+      <c r="C249" s="29"/>
+      <c r="D249" s="29"/>
+      <c r="E249" s="29"/>
+      <c r="F249" s="29"/>
+    </row>
+    <row r="250" spans="1:6">
+      <c r="A250" s="29"/>
+      <c r="B250" s="29"/>
+      <c r="C250" s="29"/>
+      <c r="D250" s="29"/>
+      <c r="E250" s="29"/>
+      <c r="F250" s="29"/>
+    </row>
+    <row r="251" spans="1:6">
+      <c r="A251" s="29"/>
+      <c r="B251" s="29"/>
+      <c r="C251" s="29"/>
+      <c r="D251" s="29"/>
+      <c r="E251" s="29"/>
+      <c r="F251" s="29"/>
+    </row>
+    <row r="252" spans="1:6">
+      <c r="A252" s="29"/>
+      <c r="B252" s="29"/>
+      <c r="C252" s="29"/>
+      <c r="D252" s="29"/>
+      <c r="E252" s="29"/>
+      <c r="F252" s="29"/>
+    </row>
+    <row r="253" spans="1:6">
+      <c r="A253" s="29"/>
+      <c r="B253" s="29"/>
+      <c r="C253" s="29"/>
+      <c r="D253" s="29"/>
+      <c r="E253" s="29"/>
+      <c r="F253" s="29"/>
+    </row>
+    <row r="254" spans="1:6">
+      <c r="A254" s="29"/>
+      <c r="B254" s="29"/>
+      <c r="C254" s="29"/>
+      <c r="D254" s="29"/>
+      <c r="E254" s="29"/>
+      <c r="F254" s="29"/>
+    </row>
+    <row r="255" spans="1:6">
+      <c r="A255" s="29"/>
+      <c r="B255" s="29"/>
+      <c r="C255" s="29"/>
+      <c r="D255" s="29"/>
+      <c r="E255" s="29"/>
+      <c r="F255" s="29"/>
+    </row>
+    <row r="256" spans="1:6">
+      <c r="A256" s="29"/>
+      <c r="B256" s="29"/>
+      <c r="C256" s="29"/>
+      <c r="D256" s="29"/>
+      <c r="E256" s="29"/>
+      <c r="F256" s="29"/>
+    </row>
+    <row r="257" spans="1:6">
+      <c r="A257" s="29"/>
+      <c r="B257" s="29"/>
+      <c r="C257" s="29"/>
+      <c r="D257" s="29"/>
+      <c r="E257" s="29"/>
+      <c r="F257" s="29"/>
+    </row>
+    <row r="258" spans="1:6">
+      <c r="A258" s="29"/>
+      <c r="B258" s="29"/>
+      <c r="C258" s="29"/>
+      <c r="D258" s="29"/>
+      <c r="E258" s="29"/>
+      <c r="F258" s="29"/>
+    </row>
+    <row r="259" spans="1:6">
+      <c r="A259" s="29"/>
+      <c r="B259" s="29"/>
+      <c r="C259" s="29"/>
+      <c r="D259" s="29"/>
+      <c r="E259" s="29"/>
+      <c r="F259" s="29"/>
+    </row>
+    <row r="260" spans="1:6">
+      <c r="A260" s="29"/>
+      <c r="B260" s="29"/>
+      <c r="C260" s="29"/>
+      <c r="D260" s="29"/>
+      <c r="E260" s="29"/>
+      <c r="F260" s="29"/>
+    </row>
+    <row r="261" spans="1:6">
+      <c r="A261" s="29"/>
+      <c r="B261" s="29"/>
+      <c r="C261" s="29"/>
+      <c r="D261" s="29"/>
+      <c r="E261" s="29"/>
+      <c r="F261" s="29"/>
+    </row>
+    <row r="262" spans="1:6">
+      <c r="A262" s="29"/>
+      <c r="B262" s="29"/>
+      <c r="C262" s="29"/>
+      <c r="D262" s="29"/>
+      <c r="E262" s="29"/>
+      <c r="F262" s="29"/>
+    </row>
+    <row r="263" spans="1:6">
+      <c r="A263" s="29"/>
+      <c r="B263" s="29"/>
+      <c r="C263" s="29"/>
+      <c r="D263" s="29"/>
+      <c r="E263" s="29"/>
+      <c r="F263" s="29"/>
+    </row>
+    <row r="264" spans="1:6">
+      <c r="A264" s="29"/>
+      <c r="B264" s="29"/>
+      <c r="C264" s="29"/>
+      <c r="D264" s="29"/>
+      <c r="E264" s="29"/>
+      <c r="F264" s="29"/>
+    </row>
+    <row r="265" spans="1:6">
+      <c r="A265" s="29"/>
+      <c r="B265" s="29"/>
+      <c r="C265" s="29"/>
+      <c r="D265" s="29"/>
+      <c r="E265" s="29"/>
+      <c r="F265" s="29"/>
+    </row>
+  </sheetData>
+  <mergeCells count="42">
+    <mergeCell ref="C50:C52"/>
+    <mergeCell ref="A53:XFD53"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="B17:B33"/>
+    <mergeCell ref="B35:B52"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="C25:C27"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="C43:C45"/>
+    <mergeCell ref="C46:C48"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="A5:B6"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="P8:P9"/>
+    <mergeCell ref="Q8:Q9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="G8:M8"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="C31:C33"/>
+    <mergeCell ref="A34:XFD34"/>
+    <mergeCell ref="B10:B15"/>
+  </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:M7 JE1:JI7 TA1:TE7 ACW1:ADA7 AMS1:AMW7 AWO1:AWS7 BGK1:BGO7 BQG1:BQK7 CAC1:CAG7 CJY1:CKC7 CTU1:CTY7 DDQ1:DDU7 DNM1:DNQ7 DXI1:DXM7 EHE1:EHI7 ERA1:ERE7 FAW1:FBA7 FKS1:FKW7 FUO1:FUS7 GEK1:GEO7 GOG1:GOK7 GYC1:GYG7 HHY1:HIC7 HRU1:HRY7 IBQ1:IBU7 ILM1:ILQ7 IVI1:IVM7 JFE1:JFI7 JPA1:JPE7 JYW1:JZA7 KIS1:KIW7 KSO1:KSS7 LCK1:LCO7 LMG1:LMK7 LWC1:LWG7 MFY1:MGC7 MPU1:MPY7 MZQ1:MZU7 NJM1:NJQ7 NTI1:NTM7 ODE1:ODI7 ONA1:ONE7 OWW1:OXA7 PGS1:PGW7 PQO1:PQS7 QAK1:QAO7 QKG1:QKK7 QUC1:QUG7 RDY1:REC7 RNU1:RNY7 RXQ1:RXU7 SHM1:SHQ7 SRI1:SRM7 TBE1:TBI7 TLA1:TLE7 TUW1:TVA7 UES1:UEW7 UOO1:UOS7 UYK1:UYO7 VIG1:VIK7 VSC1:VSG7 WBY1:WCC7 WLU1:WLY7 WVQ1:WVU7 G8 JC8 SY8 ACU8 AMQ8 AWM8 BGI8 BQE8 CAA8 CJW8 CTS8 DDO8 DNK8 DXG8 EHC8 EQY8 FAU8 FKQ8 FUM8 GEI8 GOE8 GYA8 HHW8 HRS8 IBO8 ILK8 IVG8 JFC8 JOY8 JYU8 KIQ8 KSM8 LCI8 LME8 LWA8 MFW8 MPS8 MZO8 NJK8 NTG8 ODC8 OMY8 OWU8 PGQ8 PQM8 QAI8 QKE8 QUA8 RDW8 RNS8 RXO8 SHK8 SRG8 TBC8 TKY8 TUU8 UEQ8 UOM8 UYI8 VIE8 VSA8 WBW8 WLS8 WVO8 M9 JI9 TE9 ADA9 AMW9 AWS9 BGO9 BQK9 CAG9 CKC9 CTY9 DDU9 DNQ9 DXM9 EHI9 ERE9 FBA9 FKW9 FUS9 GEO9 GOK9 GYG9 HIC9 HRY9 IBU9 ILQ9 IVM9 JFI9 JPE9 JZA9 KIW9 KSS9 LCO9 LMK9 LWG9 MGC9 MPY9 MZU9 NJQ9 NTM9 ODI9 ONE9 OXA9 PGW9 PQS9 QAO9 QKK9 QUG9 REC9 RNY9 RXU9 SHQ9 SRM9 TBI9 TLE9 TVA9 UEW9 UOS9 UYO9 VIK9 VSG9 WCC9 WLY9 WVU9">
+      <formula1>"○, ×"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P1:P9 JL1:JL9 TH1:TH9 ADD1:ADD9 AMZ1:AMZ9 AWV1:AWV9 BGR1:BGR9 BQN1:BQN9 CAJ1:CAJ9 CKF1:CKF9 CUB1:CUB9 DDX1:DDX9 DNT1:DNT9 DXP1:DXP9 EHL1:EHL9 ERH1:ERH9 FBD1:FBD9 FKZ1:FKZ9 FUV1:FUV9 GER1:GER9 GON1:GON9 GYJ1:GYJ9 HIF1:HIF9 HSB1:HSB9 IBX1:IBX9 ILT1:ILT9 IVP1:IVP9 JFL1:JFL9 JPH1:JPH9 JZD1:JZD9 KIZ1:KIZ9 KSV1:KSV9 LCR1:LCR9 LMN1:LMN9 LWJ1:LWJ9 MGF1:MGF9 MQB1:MQB9 MZX1:MZX9 NJT1:NJT9 NTP1:NTP9 ODL1:ODL9 ONH1:ONH9 OXD1:OXD9 PGZ1:PGZ9 PQV1:PQV9 QAR1:QAR9 QKN1:QKN9 QUJ1:QUJ9 REF1:REF9 ROB1:ROB9 RXX1:RXX9 SHT1:SHT9 SRP1:SRP9 TBL1:TBL9 TLH1:TLH9 TVD1:TVD9 UEZ1:UEZ9 UOV1:UOV9 UYR1:UYR9 VIN1:VIN9 VSJ1:VSJ9 WCF1:WCF9 WMB1:WMB9 WVX1:WVX9">
+      <formula1>"OK,NG,N/A"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>